<commit_message>
add get new by topic
</commit_message>
<xml_diff>
--- a/responses/test.xlsx
+++ b/responses/test.xlsx
@@ -477,27 +477,27 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hoa hậu Đỗ Mỹ Linh công khai chồng sắp cưới - VTC News</t>
+          <t>Thức khuya tàn phá sức khỏe ghê gớm, biết mà tránh kẻo hỏng gan, chóng già - VTC News</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://vtc.vn/hoa-hau-do-my-linh-cong-khai-chong-sap-cuoi-ar706895.html</t>
+          <t>https://vtc.vn/thuc-khuya-tan-pha-suc-khoe-ghe-gom-biet-ma-tranh-keo-hong-gan-chong-gia-ar706853.html</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CAIiEAjGnGuMy2xELMkWQWXQZpkqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwh5DLBg</t>
+          <t>CAIiEBkDE6UHwdl5pbX815sCoBwqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Thu, 13 Oct 2022 04:00:00 GMT</t>
+          <t>Wed, 12 Oct 2022 23:55:00 GMT</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Hoa hậu Đỗ Mỹ Linh công khai chồng sắp cưới  VTC News</t>
+          <t>Thức khuya tàn phá sức khỏe ghê gớm, biết mà tránh kẻo hỏng gan, chóng già  VTC News</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -513,27 +513,27 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Quảng Nam: Sạt lở tuyến đường huyện miền núi, 170 hộ dân bị chia cắt - VTC News</t>
+          <t>Cách ăn thịt lợn sao cho an toàn với sức khỏe - VTC News</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://vtc.vn/quang-nam-sat-lo-tuyen-duong-huyen-mien-nui-170-ho-dan-bi-chia-cat-ar706903.html</t>
+          <t>https://vtc.vn/cach-an-thit-lon-sao-cho-an-toan-voi-suc-khoe-ar706617.html</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CAIiEDSCIXZX_6lFRMd5Noj2Gl0qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEArLhw_vyMWAP3Hx2OC2TiYqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Thu, 13 Oct 2022 04:00:00 GMT</t>
+          <t>Wed, 12 Oct 2022 00:02:00 GMT</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Quảng Nam: Sạt lở tuyến đường huyện miền núi, 170 hộ dân bị chia cắt  VTC News</t>
+          <t>Cách ăn thịt lợn sao cho an toàn với sức khỏe  VTC News</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -549,27 +549,27 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hòa kịch tính Inter Milan, Barcelona dễ bị loại khỏi Cúp C1 - VTC News</t>
+          <t>Sao Việt 12/10: Bà xã Công Lý thông báo sức khỏe của chồng - VTC News</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://vtc.vn/hoa-kich-tinh-inter-milan-barcelona-de-bi-loai-khoi-cup-c1-ar706855.html</t>
+          <t>https://vtc.vn/sao-viet-12-10-ba-xa-cong-ly-thong-bao-suc-khoe-cua-chong-ar706602.html</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CAIiELt39IN16HV8f_k_aT3iuZEqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEJdsU7O0SVr_h7hcgJJFJDsqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwh5DLBg</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Thu, 13 Oct 2022 00:02:00 GMT</t>
+          <t>Tue, 11 Oct 2022 23:37:00 GMT</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Hòa kịch tính Inter Milan, Barcelona dễ bị loại khỏi Cúp C1  VTC News</t>
+          <t>Sao Việt 12/10: Bà xã Công Lý thông báo sức khỏe của chồng  VTC News</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -585,27 +585,27 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Quy trình Tổng thống Mỹ ra lệnh tiến hành một cuộc tấn công hạt nhân - VTC News</t>
+          <t>Sức khỏe bệnh nhân đầu tiên mắc đậu mùa khỉ tại Việt Nam hiện ra sao? - VTC News</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://vtc.vn/quy-trinh-tong-thong-my-ra-lenh-tien-hanh-mot-cuoc-tan-cong-hat-nhan-ar706875.html</t>
+          <t>https://vtc.vn/suc-khoe-benh-nhan-dau-tien-mac-dau-mua-khi-tai-viet-nam-hien-ra-sao-ar704877.html</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CAIiEOhM-xGEgPuZOO1AED3_fNoqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEDPllq62KY6Ykfp1_tDGTzgqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Thu, 13 Oct 2022 02:55:00 GMT</t>
+          <t>Mon, 03 Oct 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Quy trình Tổng thống Mỹ ra lệnh tiến hành một cuộc tấn công hạt nhân  VTC News</t>
+          <t>Sức khỏe bệnh nhân đầu tiên mắc đậu mùa khỉ tại Việt Nam hiện ra sao?  VTC News</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -621,27 +621,27 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Yêu cầu một trường ở Cà Mau trả lại phụ huynh 282 triệu đồng - VTC News</t>
+          <t>Bị khô miệng kéo dài gây hại thế nào với sức khỏe? - VTC News</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://vtc.vn/yeu-cau-mot-truong-o-ca-mau-tra-lai-phu-huynh-282-trieu-dong-ar706863.html</t>
+          <t>https://vtc.vn/bi-kho-mieng-keo-dai-gay-hai-the-nao-voi-suc-khoe-ar705448.html</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CAIiEIDMw-k3kz5Y_BECRFRZUmsqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwhZDLBg</t>
+          <t>CAIiEHo4G51pYh3QG_fDj_rS6x8qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Thu, 13 Oct 2022 00:57:00 GMT</t>
+          <t>Thu, 06 Oct 2022 09:13:00 GMT</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Yêu cầu một trường ở Cà Mau trả lại phụ huynh 282 triệu đồng  VTC News</t>
+          <t>Bị khô miệng kéo dài gây hại thế nào với sức khỏe?  VTC News</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -657,27 +657,27 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Dự báo thời tiết hôm nay ngày 13/10: Miền Trung, Tây Nguyên mưa to và dông - VTC News</t>
+          <t>Những lợi ích cho sức khỏe bất ngờ từ bông cải xanh - VTC News</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://vtc.vn/du-bao-thoi-tiet-hom-nay-ngay-13-10-mien-trung-tay-nguyen-mua-to-va-dong-ar706851.html</t>
+          <t>https://vtc.vn/nhung-loi-ich-cho-suc-khoe-bat-ngo-tu-bong-cai-xanh-ar705171.html</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CAIiECmhYr6SrQgLNmbIGmm2kPIqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEI1IuwkQlxkG6S3A_ZwFIsMqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwkr_sBw</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 23:41:00 GMT</t>
+          <t>Wed, 05 Oct 2022 01:33:00 GMT</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Dự báo thời tiết hôm nay ngày 13/10: Miền Trung, Tây Nguyên mưa to và dông  VTC News</t>
+          <t>Những lợi ích cho sức khỏe bất ngờ từ bông cải xanh  VTC News</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -693,27 +693,27 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Nhà Trắng công bố chiến lược an ninh quốc gia - VTC News</t>
+          <t>Tử vi 12 con giáp hôm nay thứ Sáu ngày 14/10: Tuất nên tỉnh táo, Mùi đào hoa xấu - VTC News</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://vtc.vn/nha-trang-cong-bo-chien-luoc-an-ninh-quoc-gia-ar706848.html</t>
+          <t>https://vtc.vn/tu-vi-12-con-giap-hom-nay-thu-sau-ngay-14-10-tuat-nen-tinh-tao-mui-dao-hoa-xau-ar706664.html</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CAIiED6_6pgoPCRKMsgiGSJPucAqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CBMia2h0dHBzOi8vdnRjLnZuL3R1LXZpLTEyLWNvbi1naWFwLWhvbS1uYXktdGh1LXNhdS1uZ2F5LTE0LTEwLXR1YXQtbmVuLXRpbmgtdGFvLW11aS1kYW8taG9hLXhhdS1hcjcwNjY2NC5odG1s0gFvaHR0cHM6Ly9hbXAudnRjLnZuL3R1LXZpLTEyLWNvbi1naWFwLWhvbS1uYXktdGh1LXNhdS1uZ2F5LTE0LTEwLXR1YXQtbmVuLXRpbmgtdGFvLW11aS1kYW8taG9hLXhhdS1hcjcwNjY2NC5odG1s</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 23:51:00 GMT</t>
+          <t>Thu, 13 Oct 2022 06:04:00 GMT</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Nhà Trắng công bố chiến lược an ninh quốc gia  VTC News</t>
+          <t>Tử vi 12 con giáp hôm nay thứ Sáu ngày 14/10: Tuất nên tỉnh táo, Mùi đào hoa xấu  VTC News</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -729,27 +729,27 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Nghịch cảnh đại dự án nhà ở tại Hải Phòng: Sở Tài nguyên và Môi trường nói gì? - VTC News</t>
+          <t>Cháo rất tốt cho sức khỏe nhưng tuyệt đối không được ăn theo cách này - VTC News</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://vtc.vn/nghich-canh-dai-du-an-nha-o-tai-hai-phong-so-tai-nguyen-va-moi-truong-noi-gi-ar705313.html</t>
+          <t>https://vtc.vn/chao-rat-tot-cho-suc-khoe-nhung-tuyet-doi-khong-duoc-an-theo-cach-nay-ar706397.html</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>CAIiEA_9X_KdVYwghbPvBNmPnroqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEESvTDACHICkpHRjiTnIcfkqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 23:36:00 GMT</t>
+          <t>Tue, 11 Oct 2022 03:33:58 GMT</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Nghịch cảnh đại dự án nhà ở tại Hải Phòng: Sở Tài nguyên và Môi trường nói gì?  VTC News</t>
+          <t>Cháo rất tốt cho sức khỏe nhưng tuyệt đối không được ăn theo cách này  VTC News</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -765,27 +765,27 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7 tính năng trên ô tô mà khách muốn có nhất - VTC News</t>
+          <t>Hạt vi nhựa - nỗi ám ảnh với sức khỏe con người - VTC News</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://vtc.vn/7-tinh-nang-tren-o-to-ma-khach-muon-co-nhat-ar706836.html</t>
+          <t>https://vtc.vn/hat-vi-nhua-noi-am-anh-voi-suc-khoe-con-nguoi-ar702998.html</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CAIiEMoQSHZQTMZl3lcRyOVy4Q4qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CBMiSmh0dHBzOi8vdnRjLnZuL2hhdC12aS1uaHVhLW5vaS1hbS1hbmgtdm9pLXN1Yy1raG9lLWNvbi1uZ3VvaS1hcjcwMjk5OC5odG1s0gFOaHR0cHM6Ly9hbXAudnRjLnZuL2hhdC12aS1uaHVhLW5vaS1hbS1hbmgtdm9pLXN1Yy1raG9lLWNvbi1uZ3VvaS1hcjcwMjk5OC5odG1s</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 23:13:00 GMT</t>
+          <t>Fri, 30 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>7 tính năng trên ô tô mà khách muốn có nhất  VTC News</t>
+          <t>Hạt vi nhựa - nỗi ám ảnh với sức khỏe con người  VTC News</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -801,32 +801,32 @@
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Trận địa tên lửa dưới hồ của Triều Tiên thách thức Mỹ, Hàn - VnExpress</t>
+          <t>15% người Việt Nam bị rối loạn tâm thần - VTC News</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/tran-dia-ten-lua-duoi-ho-cua-trieu-tien-thach-thuc-my-han-4522315.html</t>
+          <t>https://vtc.vn/15-nguoi-viet-nam-bi-roi-loan-tam-than-ar706274.html</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CAIiEGU4rJ-m6Ebr5JkGFTwjj04qMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw1KzYBg</t>
+          <t>CAIiEO1dweAi5iYZ80OvIPG9CwMqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 17:00:00 GMT</t>
+          <t>Mon, 10 Oct 2022 09:19:00 GMT</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Trận địa tên lửa dưới hồ của Triều Tiên thách thức Mỹ, Hàn  VnExpress</t>
+          <t>15% người Việt Nam bị rối loạn tâm thần  VTC News</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -837,27 +837,27 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Quảng Ngãi: Chó nghiệp vụ tham gia tìm kiếm người mất tích sau sạt lở thủy điện - VTC News</t>
+          <t>Ca tử vong do sốt xuất huyết cao nhất 10 năm qua, TP.HCM phân tuyến điều trị - VTC News</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://vtc.vn/quang-ngai-cho-nghiep-vu-tham-gia-tim-kiem-nguoi-mat-tich-sau-sat-lo-thuy-dien-ar706788.html</t>
+          <t>https://vtc.vn/ca-tu-vong-do-sot-xuat-huyet-cao-nhat-10-nam-qua-tp-hcm-phan-tuyen-dieu-tri-ar706838.html</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>CAIiEN3R0bDzaNE2i1kepdz5M2YqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEKgR6G6PjmVOCLomUhGLSMEqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 10:24:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:43:00 GMT</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Quảng Ngãi: Chó nghiệp vụ tham gia tìm kiếm người mất tích sau sạt lở thủy điện  VTC News</t>
+          <t>Ca tử vong do sốt xuất huyết cao nhất 10 năm qua, TP.HCM phân tuyến điều trị  VTC News</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -873,32 +873,32 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Quốc Cường Gia Lai muốn tiếp tục làm dự án trên đất công - VnExpress</t>
+          <t>Phòng cấp cứu ở TP.HCM kín trẻ mắc bệnh hô hấp - VTC News</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/quoc-cuong-gia-lai-muon-tiep-tuc-lam-du-an-tren-dat-cong-4522649.html</t>
+          <t>https://vtc.vn/phong-cap-cuu-o-tp-hcm-kin-tre-mac-benh-ho-hap-ar706858.html</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>CAIiEN3r2vYhW_qKrD6hSGm0itIqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwvM3WBg</t>
+          <t>CAIiECQoHMOq8-Xbe_DbKW3eoeEqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 12:36:06 GMT</t>
+          <t>Thu, 13 Oct 2022 00:18:00 GMT</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Quốc Cường Gia Lai muốn tiếp tục làm dự án trên đất công  VnExpress</t>
+          <t>Phòng cấp cứu ở TP.HCM kín trẻ mắc bệnh hô hấp  VTC News</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -909,27 +909,27 @@
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Hà Nội có thể sẽ bố trí xây dựng các khu nhà ở xã hội tập trung 200 - 300ha - VTC News</t>
+          <t>Bác sĩ đánh giá bị cáo Dương Thị Bạch Diệp đủ sức khỏe tham gia phiên tòa - VTC News</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://vtc.vn/ha-noi-co-the-se-bo-tri-xay-dung-cac-khu-nha-o-xa-hoi-tap-trung-200-300ha-ar706819.html</t>
+          <t>https://vtc.vn/bac-si-danh-gia-bi-cao-duong-thi-bach-diep-du-suc-khoe-tham-gia-phien-toa-ar705196.html</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>CAIiECeAL7ZZYvMv3FAm-0RVnzMqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiENDHY4OxWQOh2jlUxlR2MR8qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 12:53:00 GMT</t>
+          <t>Wed, 05 Oct 2022 04:08:00 GMT</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Hà Nội có thể sẽ bố trí xây dựng các khu nhà ở xã hội tập trung 200 - 300ha  VTC News</t>
+          <t>Bác sĩ đánh giá bị cáo Dương Thị Bạch Diệp đủ sức khỏe tham gia phiên tòa  VTC News</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -945,27 +945,27 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Chủ tịch TP.HCM: 'Điều hành xăng dầu phải không tạo cú sốc khi điều chỉnh giá' - VTC News</t>
+          <t>Ca đầu tiên trên thế giới được ghép ruột từ người ngừng tim - VTC News</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://vtc.vn/chu-tich-tp-hcm-dieu-hanh-xang-dau-phai-khong-tao-cu-soc-khi-dieu-chinh-gia-ar706824.html</t>
+          <t>https://vtc.vn/ca-dau-tien-tren-the-gioi-duoc-ghep-ruot-tu-nguoi-ngung-tim-ar706741.html</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>CAIiEJTBnyPbHrCUXN0ezcsFeUUqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEDd4UeYsf0UnJ8gO46NGw_MqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 13:18:00 GMT</t>
+          <t>Wed, 12 Oct 2022 07:38:00 GMT</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Chủ tịch TP.HCM: 'Điều hành xăng dầu phải không tạo cú sốc khi điều chỉnh giá'  VTC News</t>
+          <t>Ca đầu tiên trên thế giới được ghép ruột từ người ngừng tim  VTC News</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -981,27 +981,27 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bộ Công Thương: Nhiều DN bị tước giấy phép gây thiếu xăng dầu cục bộ - VTC News</t>
+          <t>Phê duyệt chủ trương thành lập Đại học Khoa học sức khoẻ - VTC News</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://vtc.vn/bo-cong-thuong-nhie-u-dn-bi-tuo-c-gia-y-phe-p-gay-thie-u-xang-da-u-cu-c-bo-ar706756.html</t>
+          <t>https://vtc.vn/phe-duyet-chu-truong-thanh-lap-dai-hoc-khoa-hoc-suc-khoe-ar702678.html</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>CAIiEATVwrL8P8gfYdsUV7WxI7UqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEJqhW-ginTai8O5W5XzIxu0qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 09:24:00 GMT</t>
+          <t>Fri, 23 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Bộ Công Thương: Nhiều DN bị tước giấy phép gây thiếu xăng dầu cục bộ  VTC News</t>
+          <t>Phê duyệt chủ trương thành lập Đại học Khoa học sức khoẻ  VTC News</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1017,27 +1017,27 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Ngắm nhan sắc nóng bỏng của nữ golfer đa tài - VTC News</t>
+          <t>Người có ba bộ phận này càng sạch thì càng sống thọ - VTC News</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://vtc.vn/ngam-nhan-sac-nong-bong-cua-nu-golfer-da-tai-ar706791.html</t>
+          <t>https://vtc.vn/nguoi-co-ba-bo-phan-nay-cang-sach-thi-cang-song-tho-ar706382.html</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>CAIiEHCDg1_3e41-H1P8QpVH1HcqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEIvaZlcCRk7QCG7oKnfYLQYqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 12:00:00 GMT</t>
+          <t>Tue, 11 Oct 2022 00:08:00 GMT</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Ngắm nhan sắc nóng bỏng của nữ golfer đa tài  VTC News</t>
+          <t>Người có ba bộ phận này càng sạch thì càng sống thọ  VTC News</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1053,27 +1053,27 @@
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Bộ trưởng Công Thương sẽ trực tiếp kiểm tra dự trữ xăng dầu tại TP.HCM - VTC News</t>
+          <t>Lợi ích sức khoẻ bất ngờ từ 'chuyện ấy' - VTC News</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://vtc.vn/bo-truong-cong-thuong-se-truc-tiep-kiem-tra-du-tru-xang-dau-tai-tp-hcm-ar706711.html</t>
+          <t>https://vtc.vn/loi-ich-suc-khoe-bat-ngo-tu-chuyen-ay-ar701038.html</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>CAIiEObBF3oiRqjJ_dkqG-uXwqoqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwg5DLBg</t>
+          <t>CBMiQmh0dHBzOi8vdnRjLnZuL2xvaS1pY2gtc3VjLWtob2UtYmF0LW5nby10dS1jaHV5ZW4tYXktYXI3MDEwMzguaHRtbNIBRmh0dHBzOi8vYW1wLnZ0Yy52bi9sb2ktaWNoLXN1Yy1raG9lLWJhdC1uZ28tdHUtY2h1eWVuLWF5LWFyNzAxMDM4Lmh0bWw</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 05:05:00 GMT</t>
+          <t>Thu, 15 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Bộ trưởng Công Thương sẽ trực tiếp kiểm tra dự trữ xăng dầu tại TP.HCM  VTC News</t>
+          <t>Lợi ích sức khoẻ bất ngờ từ 'chuyện ấy'  VTC News</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1089,27 +1089,27 @@
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Nissan bán mảng kinh doanh tại Nga với giá 1 euro - VTC News</t>
+          <t>Sản phẩm Thải độc gan thế hệ mới đạt Huy chương vàng vì sức khỏe cộng đồng - VTC News</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://vtc.vn/nissan-ban-mang-kinh-doanh-tai-nga-voi-gia-1-euro-ar706782.html</t>
+          <t>https://vtc.vn/san-pham-thai-doc-gan-the-he-moi-dat-huy-chuong-vang-vi-suc-khoe-cong-dong-ar705366.html</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>CAIiED9vduqy-Oa59iUSBuCA0A0qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEM7H3DyDGLfdloPx-8lI9eAqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 10:43:00 GMT</t>
+          <t>Thu, 06 Oct 2022 02:11:00 GMT</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Nissan bán mảng kinh doanh tại Nga với giá 1 euro  VTC News</t>
+          <t>Sản phẩm Thải độc gan thế hệ mới đạt Huy chương vàng vì sức khỏe cộng đồng  VTC News</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1125,27 +1125,27 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Clip 'phụ huynh khó khăn đừng theo lớp này' gây xôn xao: Phòng GD&amp;ĐT báo cáo gì? - VTC News</t>
+          <t>Đến Yoko Onsen Quang Hanh để tìm về 'suối nguồn thanh xuân' - VTC News</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://vtc.vn/clip-phu-huynh-kho-khan-dung-theo-lop-nay-gay-xon-xao-phong-gd-dt-bao-cao-gi-ar706744.html</t>
+          <t>https://vtc.vn/den-yoko-onsen-quang-hanh-de-tim-ve-suoi-nguon-thanh-xuan-ar706543.html</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>CAIiEPhsyNq-AZyMU3A-mPbOSwcqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CBMiVmh0dHBzOi8vdnRjLnZuL2Rlbi15b2tvLW9uc2VuLXF1YW5nLWhhbmgtZGUtdGltLXZlLXN1b2ktbmd1b24tdGhhbmgteHVhbi1hcjcwNjU0My5odG1s0gFaaHR0cHM6Ly9hbXAudnRjLnZuL2Rlbi15b2tvLW9uc2VuLXF1YW5nLWhhbmgtZGUtdGltLXZlLXN1b2ktbmd1b24tdGhhbmgteHVhbi1hcjcwNjU0My5odG1s</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 09:36:00 GMT</t>
+          <t>Tue, 11 Oct 2022 10:33:00 GMT</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Clip 'phụ huynh khó khăn đừng theo lớp này' gây xôn xao: Phòng GD&amp;ĐT báo cáo gì?  VTC News</t>
+          <t>Đến Yoko Onsen Quang Hanh để tìm về 'suối nguồn thanh xuân'  VTC News</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1161,27 +1161,27 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Tổng cục trưởng Tổng cục Du lịch: Cần nhìn nhận và định hình lại ngành Du lịch - VTC News</t>
+          <t>Tử vi 12 con giáp hôm nay thứ Năm ngày 13/10: Ngọ khởi sắc, Mão khó thăng tiến - VTC News</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://vtc.vn/tong-cuc-truong-tong-cuc-du-lich-can-nhin-nhan-va-dinh-hinh-lai-nganh-du-lich-ar706737.html</t>
+          <t>https://vtc.vn/tu-vi-12-con-giap-hom-nay-thu-nam-ngay-13-10-ngo-khoi-sac-mao-kho-thang-tien-ar706119.html</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>CAIiEMHVH5o1faDwmmPyLj0d23QqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwg5DLBg</t>
+          <t>CAIiEMrq_jfzg0bl5_-Ylxi37YEqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwkr_sBw</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 08:16:00 GMT</t>
+          <t>Wed, 12 Oct 2022 06:02:00 GMT</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Tổng cục trưởng Tổng cục Du lịch: Cần nhìn nhận và định hình lại ngành Du lịch  VTC News</t>
+          <t>Tử vi 12 con giáp hôm nay thứ Năm ngày 13/10: Ngọ khởi sắc, Mão khó thăng tiến  VTC News</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1197,27 +1197,27 @@
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bộ Chính trị kỷ luật 10 tổ chức đảng và 5 đảng viên từ đầu năm đến nay - VTC News</t>
+          <t>NibiAmin Gold – Bảo vệ sức khoẻ toàn diện từ các axit amin thiết yếu - VTC News</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://vtc.vn/bo-chinh-tri-ky-luat-10-to-chuc-dang-va-5-dang-vien-tu-dau-nam-den-nay-ar706706.html</t>
+          <t>https://vtc.vn/nibiamin-gold-bao-ve-suc-khoe-toan-dien-tu-cac-axit-amin-thiet-yeu-ar703919.html</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>CAIiEAjVHTMMrYgmQ1wAgSdDIHQqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww84TLBg</t>
+          <t>CAIiENQfZreBlQhT1-TTNmhxtCEqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 04:49:00 GMT</t>
+          <t>Thu, 29 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Bộ Chính trị kỷ luật 10 tổ chức đảng và 5 đảng viên từ đầu năm đến nay  VTC News</t>
+          <t>NibiAmin Gold – Bảo vệ sức khoẻ toàn diện từ các axit amin thiết yếu  VTC News</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1233,27 +1233,27 @@
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Tài khoản Facebook bị giảm lượt theo dõi, cập nhật hay là lỗi? - VTC News</t>
+          <t>Những vấn đề sức khỏe khiến bạn bị hôi miệng - VTC News</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://vtc.vn/tai-khoan-facebook-bi-giam-luot-theo-doi-cap-nhat-hay-la-loi-ar706732.html</t>
+          <t>https://vtc.vn/nhung-van-de-suc-khoe-khien-ban-bi-hoi-mieng-ar701484.html</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>CAIiEFLu-hoWrCh5hsblvzmItt4qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiELVdu9hjwwKKONZn8SATPNEqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 07:44:00 GMT</t>
+          <t>Sun, 18 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Tài khoản Facebook bị giảm lượt theo dõi, cập nhật hay là lỗi?  VTC News</t>
+          <t>Những vấn đề sức khỏe khiến bạn bị hôi miệng  VTC News</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1269,32 +1269,32 @@
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Họa sĩ đốt gần 5.000 bức tranh để 'phục vụ nghệ thuật' - VnExpress</t>
+          <t>Bayer Việt Nam tăng cường hoạt động nâng cao nhận thức về sức khoẻ sinh sản - VTC News</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/dot-gan-5-000-buc-tranh-de-chuyen-doi-nghe-thuat-4522432.html</t>
+          <t>https://vtc.vn/bayer-viet-nam-tang-cuong-hoat-dong-nang-cao-nhan-thuc-ve-suc-khoe-sinh-san-ar703244.html</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>CAIiEAj_jU1BtJlkJgp9vfJh-XYqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEFd_UvfRIS9wCQkBjhWJ7PUqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 07:48:00 GMT</t>
+          <t>Mon, 26 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Họa sĩ đốt gần 5.000 bức tranh để 'phục vụ nghệ thuật'  VnExpress</t>
+          <t>Bayer Việt Nam tăng cường hoạt động nâng cao nhận thức về sức khoẻ sinh sản  VTC News</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -1305,27 +1305,27 @@
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Triều cường cao kỷ lục, bệnh viện ở Cần Thơ lênh láng nước - VTC News</t>
+          <t>Đi trung tâm thương mại được khám bệnh và tư vấn sức khỏe miễn phí - VTC News</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://vtc.vn/anh-trieu-cuong-cao-ky-luc-benh-vien-o-can-tho-lenh-lang-nuoc-ar706662.html</t>
+          <t>https://vtc.vn/di-trung-tam-thuong-mai-duoc-kham-benh-va-tu-van-suc-khoe-mien-phi-ar701758.html</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>CAIiEEflbCNPCcTuXOhUy27Ebk8qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEJr-cEJzxLAXWPZaKw9JItwqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 04:07:00 GMT</t>
+          <t>Sun, 18 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Triều cường cao kỷ lục, bệnh viện ở Cần Thơ lênh láng nước  VTC News</t>
+          <t>Đi trung tâm thương mại được khám bệnh và tư vấn sức khỏe miễn phí  VTC News</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1341,27 +1341,27 @@
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Phía sau những dòng chữ hằn trên cơ thể người trẻ - VTC News</t>
+          <t>Ốm ai cũng biết mua thuốc, nhưng buồn thì cứ để mặc giày vò bản thân - VTC News</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://vtc.vn/phia-sau-nhung-dong-chu-han-tren-co-the-nguoi-tre-ar706718.html</t>
+          <t>https://vtc.vn/om-ai-cung-biet-mua-thuoc-nhung-buon-thi-cu-de-mac-giay-vo-ban-than-ar706206.html</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>CAIiECMt850QDjjUHWfQiRsBncUqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwkr_sBw</t>
+          <t>CAIiEEtvaCxJOHhGu0Aqnc5OCgIqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwkr_sBw</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 07:27:00 GMT</t>
+          <t>Mon, 10 Oct 2022 05:05:00 GMT</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Phía sau những dòng chữ hằn trên cơ thể người trẻ  VTC News</t>
+          <t>Ốm ai cũng biết mua thuốc, nhưng buồn thì cứ để mặc giày vò bản thân  VTC News</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1377,27 +1377,27 @@
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Á hậu Bảo Ngọc nổi bật trong phần thi bikini tại Hoa hậu Liên lục địa 2022 - VTC News</t>
+          <t>Bosugold năm thứ 3 đạt giải thưởng sản phẩm vàng - vì sức khỏe cộng đồng - VTC News</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://vtc.vn/a-hau-bao-ngoc-noi-bat-trong-phan-thi-bikini-tai-hoa-hau-lien-luc-dia-2022-ar706653.html</t>
+          <t>https://vtc.vn/bosugold-nam-thu-3-dat-giai-thuong-san-pham-vang-vi-suc-khoe-cong-dong-ar701933.html</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>CAIiEG7OL_Xb0pHk07nDUscRjWQqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwh5DLBg</t>
+          <t>CAIiEC2MZdwGO3zgYeGD4T_c1VUqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 02:46:00 GMT</t>
+          <t>Tue, 20 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Á hậu Bảo Ngọc nổi bật trong phần thi bikini tại Hoa hậu Liên lục địa 2022  VTC News</t>
+          <t>Bosugold năm thứ 3 đạt giải thưởng sản phẩm vàng - vì sức khỏe cộng đồng  VTC News</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1413,27 +1413,27 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Thống nhất trình Quốc hội cho TP.HCM thí điểm cơ chế đặc thù thêm 1 năm - VTC News</t>
+          <t>Áo ngực có phải nguyên nhân gây ung thư vú? - VTC News</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://vtc.vn/thong-nhat-trinh-quoc-hoi-cho-tp-hcm-thi-diem-co-che-dac-thu-them-1-nam-ar706700.html</t>
+          <t>https://vtc.vn/ao-nguc-co-phai-nguyen-nhan-gay-ung-thu-vu-ar706840.html</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>CAIiEG2AQAyLWdgt3Ul3-F1jybgqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEFmpd_wKJfT7rbrs0Tj4_BQqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 04:35:00 GMT</t>
+          <t>Wed, 12 Oct 2022 23:32:00 GMT</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Thống nhất trình Quốc hội cho TP.HCM thí điểm cơ chế đặc thù thêm 1 năm  VTC News</t>
+          <t>Áo ngực có phải nguyên nhân gây ung thư vú?  VTC News</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1449,27 +1449,27 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Nhận định bóng đá Rangers vs Liverpool vòng bảng Cúp C1 - VTC News</t>
+          <t>12 cách sử dụng hóa chất đảm bảo an toàn sức khỏe, tránh gây hỏng đồ đạc - VTC News</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://vtc.vn/nhan-dinh-bong-da-rangers-vs-liverpool-vong-bang-cup-c1-ar706630.html</t>
+          <t>https://vtc.vn/12-cach-su-dung-hoa-chat-dam-bao-an-toan-suc-khoe-tranh-gay-hong-do-dac-ar704939.html</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>CAIiEC496TR9YO0Dc1gmUIcI6dAqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiELHkFtzev1AnIDeUD1Z8GnsqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 00:28:00 GMT</t>
+          <t>Tue, 04 Oct 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Nhận định bóng đá Rangers vs Liverpool vòng bảng Cúp C1  VTC News</t>
+          <t>12 cách sử dụng hóa chất đảm bảo an toàn sức khỏe, tránh gây hỏng đồ đạc  VTC News</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1485,27 +1485,27 @@
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Trường học xin lỗi vì để học sinh bị dị ứng thuốc diệt muỗi, phụ huynh lên tiếng - VTC News</t>
+          <t>Nova Service hợp tác cùng Mega Gangnam trong lĩnh vực chăm sóc sức khoẻ, thẩm mỹ - VTC News</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://vtc.vn/truong-hoc-xin-loi-vi-de-hoc-sinh-bi-di-ung-thuoc-diet-muoi-phu-huynh-len-tieng-ar706586.html</t>
+          <t>https://vtc.vn/nova-service-hop-tac-cung-mega-gangnam-trong-linh-vuc-cham-soc-suc-khoe-tham-my-ar704018.html</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>CAIiEPpU8JJqPmuXsdq90GeayXcqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwhZDLBg</t>
+          <t>CAIiEB9wdHMf6GCvh5PWqGrHhoEqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 01:01:00 GMT</t>
+          <t>Sat, 01 Oct 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Trường học xin lỗi vì để học sinh bị dị ứng thuốc diệt muỗi, phụ huynh lên tiếng  VTC News</t>
+          <t>Nova Service hợp tác cùng Mega Gangnam trong lĩnh vực chăm sóc sức khoẻ, thẩm mỹ  VTC News</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1521,32 +1521,32 @@
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Nghe podcasts | Điểm tin 11h: Metro Số 2 hơn một thập kỷ lận đận; Thẩm phán Nga thiệt mạng trong vụ nổ cầu Crimea - VnExpress</t>
+          <t>Dí dỏm, hài hước qua bộ ảnh 'Già có gì vui' ở viện dưỡng lão - VTC News</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/diem-tin-6h-nhieu-cua-hang-o-tp-hcm-van-thieu-xang-ukraine-tuyen-bo-ha-hon-30-ten-lua-uav-nga-4522248.html</t>
+          <t>https://vtc.vn/di-dom-hai-huoc-qua-bo-anh-gia-co-gi-vui-o-vien-duong-lao-ar706620.html</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>CAIiEEiRvelc6VwEBWqPFqzhqcoqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiECp4xwylQajV-kooQLN0ie4qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwkr_sBw</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 23:00:00 GMT</t>
+          <t>Wed, 12 Oct 2022 04:19:00 GMT</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Nghe podcasts | Điểm tin 11h: Metro Số 2 hơn một thập kỷ lận đận; Thẩm phán Nga thiệt mạng trong vụ nổ cầu Crimea  VnExpress</t>
+          <t>Dí dỏm, hài hước qua bộ ảnh 'Già có gì vui' ở viện dưỡng lão  VTC News</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -1557,27 +1557,27 @@
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Người dân Quy Nhơn chèo thuyền giữa phố - VTC News</t>
+          <t>Nam sinh 18 tuổi trầm cảm, muốn tự sát do kỳ vọng của bố mẹ - VTC News</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://vtc.vn/nguoi-dan-quy-nhon-cheo-thuyen-giua-pho-ar706583.html</t>
+          <t>https://vtc.vn/nam-sinh-18-tuoi-tram-cam-muon-tu-sat-do-ky-vong-cua-bo-me-ar706640.html</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>CAIiEAWIXpur82wErTdcLbfybOsqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEH-3p1dfN8b-7b5hl9-ffLUqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:15:00 GMT</t>
+          <t>Wed, 12 Oct 2022 07:55:00 GMT</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Người dân Quy Nhơn chèo thuyền giữa phố  VTC News</t>
+          <t>Nam sinh 18 tuổi trầm cảm, muốn tự sát do kỳ vọng của bố mẹ  VTC News</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1593,27 +1593,27 @@
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>HLV Kiatisak sẽ từ chối tuyển Thái Lan để ở lại với bầu Đức? - VTC News</t>
+          <t>Ai không nên ăn quả hồng? - VTC News</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://vtc.vn/hlv-kiatisak-se-tu-choi-tuyen-thai-lan-de-o-lai-voi-bau-duc-ar706589.html</t>
+          <t>https://vtc.vn/ai-khong-nen-an-qua-hong-ar706337.html</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>CAIiEMyrhjArMa1J5dWqSegdD9wqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6ZDLBg</t>
+          <t>CAIiEFg9rQsMs2roNdyw6zLsLUUqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:19:00 GMT</t>
+          <t>Wed, 12 Oct 2022 00:09:00 GMT</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>HLV Kiatisak sẽ từ chối tuyển Thái Lan để ở lại với bầu Đức?  VTC News</t>
+          <t>Ai không nên ăn quả hồng?  VTC News</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1629,27 +1629,27 @@
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Thêm 4 chương trình đào tạo của Học viện Báo chí và Tuyên truyền được kiểm định - VTC News</t>
+          <t>Bộ Y tế ra mắt Sổ Mẹ và Bé phiên bản điện tử - VTC News</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://vtc.vn/them-4-chuong-trinh-dao-tao-cua-hoc-vien-bao-chi-va-tuyen-truyen-duoc-kiem-dinh-ar706518.html</t>
+          <t>https://vtc.vn/bo-y-te-ra-mat-so-me-va-be-phien-ban-dien-tu-ar702418.html</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>CAIiEIuailhfkvznJmsWyCtk-n4qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwhZDLBg</t>
+          <t>CAIiEGM2N2ttfanh9j0H-bOjGcoqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 07:18:00 GMT</t>
+          <t>Thu, 22 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Thêm 4 chương trình đào tạo của Học viện Báo chí và Tuyên truyền được kiểm định  VTC News</t>
+          <t>Bộ Y tế ra mắt Sổ Mẹ và Bé phiên bản điện tử  VTC News</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1665,27 +1665,27 @@
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Bổ nhiệm hai Phó Tổng Giám đốc Bảo hiểm Xã hội Việt Nam - VTC News</t>
+          <t>Nutifood trở thành ông chủ mới của thương hiệu sức khỏe châu Âu - VTC News</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://vtc.vn/bo-nhiem-hai-pho-tong-giam-doc-bao-hiem-xa-hoi-viet-nam-ar706582.html</t>
+          <t>https://vtc.vn/nutifood-tro-thanh-ong-chu-moi-cua-thuong-hieu-suc-khoe-chau-au-ar701772.html</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>CAIiEI-QCSaZA3266MFRtlcZA-kqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiENqRB6OiShRHaevaKFapj5oqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwg5DLBg</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:39:00 GMT</t>
+          <t>Mon, 19 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Bổ nhiệm hai Phó Tổng Giám đốc Bảo hiểm Xã hội Việt Nam  VTC News</t>
+          <t>Nutifood trở thành ông chủ mới của thương hiệu sức khỏe châu Âu  VTC News</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1701,27 +1701,27 @@
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Lịch thi đấu bóng đá hôm nay 12/10 và ngày mai 13/10 - VTC News</t>
+          <t>Hà Nội ô nhiễm không khí ở ngưỡng rất xấu - VTC News</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://vtc.vn/lich-thi-dau-bong-da-hom-nay-12-10-va-ngay-mai-13-10-ar706578.html</t>
+          <t>https://vtc.vn/ha-noi-o-nhiem-khong-khi-o-nguong-rat-xau-ar706446.html</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>CAIiECDSo6OOMqXzPdVZJLenvRMqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEGmH1RaNmVbDMNCvwdc8TasqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:20:00 GMT</t>
+          <t>Tue, 11 Oct 2022 04:08:00 GMT</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Lịch thi đấu bóng đá hôm nay 12/10 và ngày mai 13/10  VTC News</t>
+          <t>Hà Nội ô nhiễm không khí ở ngưỡng rất xấu  VTC News</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1737,27 +1737,27 @@
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Máy bay Vietnam Airlines bị sét đánh thủng vỏ - VTC News</t>
+          <t>Mô hình 'Trường học Xanh - Sạch - Khỏe' được triển khai trên toàn quốc - VTC News</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://vtc.vn/may-bay-vietnam-airlines-bi-set-danh-thung-vo-ar706535.html</t>
+          <t>https://vtc.vn/mo-hinh-truong-hoc-xanh-sach-khoe-duoc-trien-khai-tren-toan-quoc-ar706291.html</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>CAIiEDQ3iTVFBIExZ-B_vqNzhp8qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwg5DLBg</t>
+          <t>CAIiEFJhXxYsEBpatQIBuPQTKVUqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 09:11:00 GMT</t>
+          <t>Mon, 10 Oct 2022 11:00:00 GMT</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Máy bay Vietnam Airlines bị sét đánh thủng vỏ  VTC News</t>
+          <t>Mô hình 'Trường học Xanh - Sạch - Khỏe' được triển khai trên toàn quốc  VTC News</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1773,27 +1773,27 @@
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Truy bắt hung thủ sát hại 1 phụ nữ đơn thân - VTC News</t>
+          <t>Cả đời cực khổ, cụ bà U90 quyết dành hết tiền để du lịch thế giới một mình - VTC News</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://vtc.vn/truy-bat-hung-thu-sat-hai-1-phu-nu-don-than-ar706415.html</t>
+          <t>https://vtc.vn/ca-doi-cuc-kho-cu-ba-u90-quyet-danh-het-tien-de-du-lich-the-gioi-mot-minh-ar705499.html</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>CAIiEPC2XPC1wVXXU_2Z5nmLiDQqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CBMiZmh0dHBzOi8vdnRjLnZuL2NhLWRvaS1jdWMta2hvLWN1LWJhLXU5MC1xdXlldC1kYW5oLWhldC10aWVuLWRlLWR1LWxpY2gtdGhlLWdpb2ktbW90LW1pbmgtYXI3MDU0OTkuaHRtbNIBamh0dHBzOi8vYW1wLnZ0Yy52bi9jYS1kb2ktY3VjLWtoby1jdS1iYS11OTAtcXV5ZXQtZGFuaC1oZXQtdGllbi1kZS1kdS1saWNoLXRoZS1naW9pLW1vdC1taW5oLWFyNzA1NDk5Lmh0bWw</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 03:34:00 GMT</t>
+          <t>Wed, 12 Oct 2022 09:30:00 GMT</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Truy bắt hung thủ sát hại 1 phụ nữ đơn thân  VTC News</t>
+          <t>Cả đời cực khổ, cụ bà U90 quyết dành hết tiền để du lịch thế giới một mình  VTC News</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -1809,27 +1809,27 @@
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Nhận định bóng đá AC Milan vs Chelsea vòng bảng Cúp C1 châu Âu - VTC News</t>
+          <t>Tìm người thân cho bé trai 10 ngày tuổi bị bỏ rơi trong thùng giấy ở Đồng Nai - VTC News</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://vtc.vn/nhan-dinh-bong-da-ac-milan-vs-chelsea-vong-bang-cup-c1-chau-au-ar706378.html</t>
+          <t>https://vtc.vn/tim-nguoi-than-cho-be-trai-10-ngay-tuoi-bi-bo-roi-trong-thung-giay-o-dong-nai-ar706920.html</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>CAIiEBg09nfr7KX5ZZL7h4xcyKwqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEE0csiWj_E7Se5ARntit_BMqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww84TLBg</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 00:30:00 GMT</t>
+          <t>Thu, 13 Oct 2022 05:39:00 GMT</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Nhận định bóng đá AC Milan vs Chelsea vòng bảng Cúp C1 châu Âu  VTC News</t>
+          <t>Tìm người thân cho bé trai 10 ngày tuổi bị bỏ rơi trong thùng giấy ở Đồng Nai  VTC News</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -1845,27 +1845,27 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Nhạc sĩ Phương Uyên: 'Tôi dễ bị tổn thương và thích sống ẩn dật' - VTC News</t>
+          <t>Cầm bút, đeo kính rồi vẫn loanh quanh đi tìm, cẩn thận sa sút trí tuệ - VTC News</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://vtc.vn/nhac-si-phuong-uyen-toi-de-bi-ton-thuong-va-thich-song-an-dat-ar706404.html</t>
+          <t>https://vtc.vn/cam-but-deo-kinh-roi-van-loanh-quanh-di-tim-can-than-sa-sut-tri-tue-ar706651.html</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>CAIiEHGPTUbP5jpIqx6EHX1ejcwqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwh5DLBg</t>
+          <t>CAIiEJIWYVQf5x9om0CaRQwYC1AqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 03:30:00 GMT</t>
+          <t>Wed, 12 Oct 2022 04:35:00 GMT</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Nhạc sĩ Phương Uyên: 'Tôi dễ bị tổn thương và thích sống ẩn dật'  VTC News</t>
+          <t>Cầm bút, đeo kính rồi vẫn loanh quanh đi tìm, cẩn thận sa sút trí tuệ  VTC News</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -1881,27 +1881,27 @@
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Cây xăng khan hàng, khách chật vật mua: Bộ Công Thương có biện pháp gì? - VTC News</t>
+          <t>Máy bay của Vietnam Airlines phải quay đầu để cấp cứu hành khách - VTC News</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://vtc.vn/cay-xang-khan-ha-ng-kha-ch-cha-t-va-t-mua-bo-cong-thuong-co-bien-phap-gi-ar706275.html</t>
+          <t>https://vtc.vn/may-bay-cua-vietnam-airlines-phai-quay-dau-de-cap-cuu-hanh-khach-ar705883.html</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>CAIiEK81fX-t_GxnSj4NrSFefScqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEBY9GUZHub0g7yCS173vobEqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 08:48:00 GMT</t>
+          <t>Sat, 08 Oct 2022 09:50:00 GMT</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Cây xăng khan hàng, khách chật vật mua: Bộ Công Thương có biện pháp gì?  VTC News</t>
+          <t>Máy bay của Vietnam Airlines phải quay đầu để cấp cứu hành khách  VTC News</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -1917,32 +1917,32 @@
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Aubameyang: 'Arteta không thể quản lý các ngôi sao' - VnExpress</t>
+          <t>Đỗ Vinh Quang: Doanh nhân trẻ với tinh thần trách nhiệm xã hội - VTC News</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/aubameyang-che-arteta-khong-biet-dan-dat-cau-thu-lon-4521744.html</t>
+          <t>https://vtc.vn/do-vinh-quang-doanh-nhan-tre-voi-tinh-than-trach-nhiem-xa-hoi-ar706870.html</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>CAIiEMQRXLF0OZMNCXaXi-x02g0qMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwu83WBg</t>
+          <t>CAIiEKLBziqQ44ddtF6z8HHxF9IqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 23:31:00 GMT</t>
+          <t>Thu, 13 Oct 2022 01:41:00 GMT</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Aubameyang: 'Arteta không thể quản lý các ngôi sao'  VnExpress</t>
+          <t>Đỗ Vinh Quang: Doanh nhân trẻ với tinh thần trách nhiệm xã hội  VTC News</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -1953,27 +1953,27 @@
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Voi hoang dã chặn đầu ô tô trên cao tốc ở Thái Lan - VTC News</t>
+          <t>4 ‘thêm’, 3 ‘bớt’ vào buổi sáng giúp tránh xa bệnh tật - VTC News</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://vtc.vn/video-voi-hoang-da-chan-dau-o-to-tren-cao-toc-o-thai-lan-ar706528.html</t>
+          <t>https://vtc.vn/4-them-3-bot-vao-buoi-sang-giup-tranh-xa-benh-tat-ar701661.html</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>CAIiEILXUAFQF-7nSZQWx51TLO8qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiELN-2gu3lBP0gGWtsYxJq5EqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 00:31:19 GMT</t>
+          <t>Mon, 19 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Voi hoang dã chặn đầu ô tô trên cao tốc ở Thái Lan  VTC News</t>
+          <t>4 ‘thêm’, 3 ‘bớt’ vào buổi sáng giúp tránh xa bệnh tật  VTC News</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -1989,27 +1989,27 @@
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ảnh: Hiện trạng vườn hoa Con Cóc 120 tuổi trước ngày 'thay áo mới' - VTC News</t>
+          <t>Cánh rừng ngập mặn ở Hải Phòng chết khô: Quận và Sở đẩy trách nhiệm cho nhau - VTC News</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://vtc.vn/anh-hien-trang-vuon-hoa-con-coc-120-tuoi-truoc-ngay-thay-ao-moi-ar705666.html</t>
+          <t>https://vtc.vn/canh-rung-ngap-man-o-hai-phong-chet-kho-quan-va-so-day-trach-nhiem-cho-nhau-ar706771.html</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>CAIiECQ72xLiy_GFe1NvgS1EimMqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEAdC4H53y094NSzPs7HSprkqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww84TLBg</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 00:00:00 GMT</t>
+          <t>Thu, 13 Oct 2022 06:30:00 GMT</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Ảnh: Hiện trạng vườn hoa Con Cóc 120 tuổi trước ngày 'thay áo mới'  VTC News</t>
+          <t>Cánh rừng ngập mặn ở Hải Phòng chết khô: Quận và Sở đẩy trách nhiệm cho nhau  VTC News</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2025,27 +2025,27 @@
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MC Liêu Hà Trinh nói lời ngôn tình với chồng doanh nhân trong đám cưới - VTC News</t>
+          <t>Những sai lầm khi nấu ăn có thể gây ung thư mà đa phần người Việt đều mắc phải - VTC News</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://vtc.vn/mc-lieu-ha-trinh-noi-loi-ngon-tinh-voi-chong-doanh-nhan-trong-dam-cuoi-ar706343.html</t>
+          <t>https://vtc.vn/nhung-sai-lam-khi-nau-an-co-the-gay-ung-thu-ma-da-phan-nguoi-viet-deu-mac-phai-ar704543.html</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>CAIiEE56RSzNfRthJOTGRflvT1sqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEMqqmdDb-DVwBA0ECVgJpSsqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 15:46:00 GMT</t>
+          <t>Sun, 02 Oct 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>MC Liêu Hà Trinh nói lời ngôn tình với chồng doanh nhân trong đám cưới  VTC News</t>
+          <t>Những sai lầm khi nấu ăn có thể gây ung thư mà đa phần người Việt đều mắc phải  VTC News</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2061,27 +2061,27 @@
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Điều tra vụ cô gái tử vong bên cạnh nam thanh niên bị thương nặng ở Hải Dương - VTC News</t>
+          <t>5 loại thực phẩm hủy hoại đời sống tình dục của bạn - VTC News</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://vtc.vn/dieu-tra-vu-co-gai-tu-vong-ben-canh-nam-thanh-nien-bi-thuong-nang-o-hai-duong-ar706355.html</t>
+          <t>https://vtc.vn/5-loai-thuc-pham-huy-hoai-doi-song-tinh-duc-cua-ban-ar701964.html</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>CAIiEB-LYjj4dqyDNOLgr57kGTgqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEEWuVTnmNPCspvOmZcedNQAqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 15:30:00 GMT</t>
+          <t>Tue, 20 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Điều tra vụ cô gái tử vong bên cạnh nam thanh niên bị thương nặng ở Hải Dương  VTC News</t>
+          <t>5 loại thực phẩm hủy hoại đời sống tình dục của bạn  VTC News</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2097,27 +2097,27 @@
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
         <is>
-          <t>TikTok cập nhật thêm các tính năng an toàn - VTC News</t>
+          <t>Tử vi 12 cung hoàng đạo ngày 5/10: Bảo Bình đừng sợ hãi, Bọ Cạp vạn sự như ý - VTC News</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://vtc.vn/tiktok-cap-nhat-them-cac-tinh-nang-an-toan-ar706350.html</t>
+          <t>https://vtc.vn/tu-vi-12-cung-hoang-dao-ngay-5-10-bao-binh-dung-so-hai-bo-cap-van-su-nhu-y-ar704565.html</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>CAIiEN9-F-Tey5FUN6rDUkEFe2MqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiELWgNxz_Ox144vConc0zwCIqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwkr_sBw</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 14:45:00 GMT</t>
+          <t>Tue, 04 Oct 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>TikTok cập nhật thêm các tính năng an toàn  VTC News</t>
+          <t>Tử vi 12 cung hoàng đạo ngày 5/10: Bảo Bình đừng sợ hãi, Bọ Cạp vạn sự như ý  VTC News</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2133,27 +2133,27 @@
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Bộ trưởng Hồ Đức Phớc: Doanh nghiệp phát hành trái phiếu cam kết trả đúng hạn - VTC News</t>
+          <t>Điểm chuẩn các trường ngành Y Dược có thể giảm từ 0,5 đến 1,5 điểm - VTC News</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://vtc.vn/bo-truong-ho-duc-phoc-doanh-nghiep-phat-hanh-trai-phieu-cam-ket-tra-dung-han-ar706334.html</t>
+          <t>https://vtc.vn/diem-chuan-cac-truong-nganh-y-duoc-co-the-giam-tu-0-5-den-1-5-diem-ar700823.html</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>CAIiEJ-jygUknfcIpgJ4lSCF2-YqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEKnRiydBgik5ks-IkHspZhkqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwhZDLBg</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 13:06:00 GMT</t>
+          <t>Thu, 15 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Bộ trưởng Hồ Đức Phớc: Doanh nghiệp phát hành trái phiếu cam kết trả đúng hạn  VTC News</t>
+          <t>Điểm chuẩn các trường ngành Y Dược có thể giảm từ 0,5 đến 1,5 điểm  VTC News</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2169,27 +2169,27 @@
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Phương Anh Đào - Hoàng Trung gây chú ý tại lễ ra mắt 'Bếp Trưởng Tới!' - VTC News</t>
+          <t>Toàn văn phát biểu của Tổng Bí thư Nguyễn Phú Trọng tại Hội nghị TW 6 khoá XIII - VTC News</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://vtc.vn/phuong-anh-dao-hoang-trung-gay-chu-y-tai-le-ra-mat-bep-truong-toi-ar706344.html</t>
+          <t>https://vtc.vn/toan-van-phat-bieu-cua-tong-bi-thu-nguyen-phu-trong-tai-hoi-nghi-tw-6-khoa-xiii-ar704835.html</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>CAIiEHz5FP6zYUiTcf3GnRS0GlcqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
+          <t>CAIiEOhXYDQXuqCEp-j1YUvGZxcqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 14:16:00 GMT</t>
+          <t>Mon, 03 Oct 2022 08:35:00 GMT</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Phương Anh Đào - Hoàng Trung gây chú ý tại lễ ra mắt 'Bếp Trưởng Tới!'  VTC News</t>
+          <t>Toàn văn phát biểu của Tổng Bí thư Nguyễn Phú Trọng tại Hội nghị TW 6 khoá XIII  VTC News</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2205,32 +2205,32 @@
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Ông Putin tố Ukraine 'tấn công khủng bố cầu Crimea' - VnExpress</t>
+          <t>Tạm giữ hình sự người chồng chém đứt lìa 2 cánh tay vợ ở Đồng Nai - VTC News</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ong-putin-to-ukraine-dung-sau-vu-no-cau-crimea-4521139.html</t>
+          <t>https://vtc.vn/tam-giu-hinh-su-nguoi-chong-chem-dut-lia-2-canh-tay-vo-o-dong-nai-ar700847.html</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>CAIiEJcAO_bjxzSXVcd3A6Bu2QgqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwuM3WBg</t>
+          <t>CAIiEFfL2NPLZnMMzTfe7xstrOsqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Sun, 09 Oct 2022 23:35:00 GMT</t>
+          <t>Thu, 15 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Ông Putin tố Ukraine 'tấn công khủng bố cầu Crimea'  VnExpress</t>
+          <t>Tạm giữ hình sự người chồng chém đứt lìa 2 cánh tay vợ ở Đồng Nai  VTC News</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2241,27 +2241,27 @@
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Ba địa phương cho học sinh tạm nghỉ do triều cường, ngập lụt - VTC News</t>
+          <t>Các lợi ích sức khoẻ tiềm năng khi châm cứu - VTC News</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://vtc.vn/ba-dia-phuong-cho-hoc-sinh-tam-nghi-do-trieu-cuong-ngap-lut-ar706259.html</t>
+          <t>https://vtc.vn/cac-loi-ich-suc-khoe-tiem-nang-khi-cham-cuu-ar694775.html</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>CAIiENVb9bFci4Bj2gx2w05jaW8qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwhZDLBg</t>
+          <t>CBMiSGh0dHBzOi8vdnRjLnZuL2NhYy1sb2ktaWNoLXN1Yy1raG9lLXRpZW0tbmFuZy1raGktY2hhbS1jdXUtYXI2OTQ3NzUuaHRtbNIBTGh0dHBzOi8vYW1wLnZ0Yy52bi9jYWMtbG9pLWljaC1zdWMta2hvZS10aWVtLW5hbmcta2hpLWNoYW0tY3V1LWFyNjk0Nzc1Lmh0bWw</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 08:10:00 GMT</t>
+          <t>Tue, 16 Aug 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Ba địa phương cho học sinh tạm nghỉ do triều cường, ngập lụt  VTC News</t>
+          <t>Các lợi ích sức khoẻ tiềm năng khi châm cứu  VTC News</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2277,27 +2277,27 @@
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Thị trường bất động sản Phổ Yên trước hiệu ứng ‘từ quê lên phố’ - VTC News</t>
+          <t>10 thiết bị chăm sóc sức khỏe cha mẹ tuổi già - VTC News</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://vtc.vn/thi-truong-bat-dong-san-pho-yen-truoc-hieu-ung-tu-que-len-pho-ar705705.html</t>
+          <t>https://vtc.vn/10-thiet-bi-cham-soc-suc-khoe-cha-me-tuoi-gia-ar692538.html</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>CBMiWmh0dHBzOi8vdnRjLnZuL3RoaS10cnVvbmctYmF0LWRvbmctc2FuLXBoby15ZW4tdHJ1b2MtaGlldS11bmctdHUtcXVlLWxlbi1waG8tYXI3MDU3MDUuaHRtbNIBXmh0dHBzOi8vYW1wLnZ0Yy52bi90aGktdHJ1b25nLWJhdC1kb25nLXNhbi1waG8teWVuLXRydW9jLWhpZXUtdW5nLXR1LXF1ZS1sZW4tcGhvLWFyNzA1NzA1Lmh0bWw</t>
+          <t>CAIiEPHh_zOklnfug512AI34f1YqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 05:08:00 GMT</t>
+          <t>Fri, 05 Aug 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Thị trường bất động sản Phổ Yên trước hiệu ứng ‘từ quê lên phố’  VTC News</t>
+          <t>10 thiết bị chăm sóc sức khỏe cha mẹ tuổi già  VTC News</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2313,32 +2313,32 @@
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Miền Trung mưa lớn, nhiều thủy điện xả lũ - VnExpress</t>
+          <t>Dàn người đẹp Hoa khôi Nam Bộ khoe hình thể khi trình diễn bikini - VTC News</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/thuy-dien-lon-nhat-thua-thien-hue-xa-lu-4521229.html</t>
+          <t>https://vtc.vn/dan-nguoi-dep-hoa-khoi-nam-bo-khoe-hinh-the-khi-trinh-dien-bikini-ar706005.html</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>CAIiEKIf4QvMJG-akF4Akxyl13oqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEM-cDdRjs-2pBGQWKLkwi1kqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwh5DLBg</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 04:46:37 GMT</t>
+          <t>Sun, 09 Oct 2022 06:13:00 GMT</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Miền Trung mưa lớn, nhiều thủy điện xả lũ  VnExpress</t>
+          <t>Dàn người đẹp Hoa khôi Nam Bộ khoe hình thể khi trình diễn bikini  VTC News</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2349,32 +2349,32 @@
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Bố mẹ bị phạt vì để con gái 5 tuổi lái xe hơi - Ngôi Sao</t>
+          <t>Chuyên gia bật mí bí quyết bảo vệ sức khoẻ cho người làm ca đêm - VTC News</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>https://ngoisao.vnexpress.net/bo-me-bi-phat-vi-de-con-gai-5-tuoi-lai-xe-hoi-4521184.html</t>
+          <t>https://vtc.vn/chuyen-gia-bat-mi-bi-quyet-bao-ve-suc-khoe-cho-nguoi-lam-ca-dem-ar696041.html</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>CAIiEHkreXf9nkr3mq64YYwpbGAqMwgEKioIACIQyq3Fh2mV-aXM5A3HYfBoBioUCAoiEMqtxYdplfmlzOQNx2HwaAYwsKvYBg</t>
+          <t>CBMiXGh0dHBzOi8vdnRjLnZuL2NodXllbi1naWEtYmF0LW1pLWJpLXF1eWV0LWJhby12ZS1zdWMta2hvZS1jaG8tbmd1b2ktbGFtLWNhLWRlbS1hcjY5NjA0MS5odG1s0gEA</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 04:55:41 GMT</t>
+          <t>Mon, 22 Aug 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Bố mẹ bị phạt vì để con gái 5 tuổi lái xe hơi  Ngôi Sao</t>
+          <t>Chuyên gia bật mí bí quyết bảo vệ sức khoẻ cho người làm ca đêm  VTC News</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Ngôi Sao</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2385,32 +2385,32 @@
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Làm rõ trách nhiệm các bên liên quan dự án BOT - VnExpress</t>
+          <t>Sao Việt 22/9: Nghe lời chồng, Ngô Thanh Vân thỏa sức phơi nắng ở biển - VTC News</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/de-nghi-lam-ro-trach-nhiem-cac-ben-lien-quan-du-an-bot-4521282.html</t>
+          <t>https://vtc.vn/sao-viet-22-9-nghe-loi-chong-ngo-thanh-van-thoa-suc-phoi-nang-o-bien-ar702311.html</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>CAIiENIC9d9yWs6k-6e4SC_037IqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEFKr7RS6vGS-1wxbzRR94asqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 05:00:59 GMT</t>
+          <t>Thu, 22 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Làm rõ trách nhiệm các bên liên quan dự án BOT  VnExpress</t>
+          <t>Sao Việt 22/9: Nghe lời chồng, Ngô Thanh Vân thỏa sức phơi nắng ở biển  VTC News</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2421,32 +2421,32 @@
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Cháy năm ca nô du lịch ở bến Cửa Đại - VnExpress</t>
+          <t>Sức khỏe của Nữ hoàng Anh 'đáng lo ngại' - VTC News</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/chay-nam-cano-du-lich-o-ben-cua-dai-4521161.html</t>
+          <t>https://vtc.vn/suc-khoe-cua-nu-hoang-anh-dang-lo-ngai-ar699498.html</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>CAIiEOdin18B0vjNfhun_VtbjwYqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEDfiD7XXL70z2-uLS5uNk4MqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwhJDLBg</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 02:11:28 GMT</t>
+          <t>Thu, 08 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Cháy năm ca nô du lịch ở bến Cửa Đại  VnExpress</t>
+          <t>Sức khỏe của Nữ hoàng Anh 'đáng lo ngại'  VTC News</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2457,32 +2457,32 @@
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Nghe podcasts | Điểm tin 17h: Nổ lớn ở Kiev; Chứng khoán đảo chiều tăng - VnExpress</t>
+          <t>Nghi ngại về sức khỏe của Tổng thống Biden - VTC News</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/diem-tin-17h-no-lon-o-kiev-chung-khoan-dao-chieu-tang-4521138.html</t>
+          <t>https://vtc.vn/nghi-ngai-ve-suc-khoe-cua-tong-thong-biden-ar684437.html</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>CBMiWGh0dHBzOi8vdm5leHByZXNzLm5ldC9kaWVtLXRpbi0xN2gtbm8tbG9uLW8ta2lldi1jaHVuZy1raG9hbi1kYW8tY2hpZXUtdGFuZy00NTIxMTM4Lmh0bWzSAQA</t>
+          <t>CAIiENkKOeMsmLDI_fEj-1eY_LAqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 10:03:11 GMT</t>
+          <t>Tue, 28 Jun 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Nghe podcasts | Điểm tin 17h: Nổ lớn ở Kiev; Chứng khoán đảo chiều tăng  VnExpress</t>
+          <t>Nghi ngại về sức khỏe của Tổng thống Biden  VTC News</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2493,32 +2493,32 @@
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Ai trả tiền trái phiếu? - VnExpress</t>
+          <t>Chăm sóc sức khỏe tâm thần trong trường học: Không thể trì hoãn - VTC News</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ai-tra-tien-trai-phieu-4521047.html</t>
+          <t>https://vtc.vn/cham-soc-suc-khoe-tam-than-trong-truong-hoc-khong-the-tri-hoan-ar674391.html</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>CAIiEIH80trm2k58nR8lwI57W0IqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEG1-ziMbPw4wm_aFPQ9Qig4qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwhZDLBg</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Sun, 09 Oct 2022 17:00:00 GMT</t>
+          <t>Mon, 02 May 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Ai trả tiền trái phiếu?  VnExpress</t>
+          <t>Chăm sóc sức khỏe tâm thần trong trường học: Không thể trì hoãn  VTC News</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2529,27 +2529,27 @@
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Vẻ đẹp kiêu sa của nữ diễn viên vướng tin đồn hẹn hò Iker Casillas - VTC News</t>
+          <t>12 tác hại của đồ ăn nhanh với sức khỏe - VTC News</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>https://vtc.vn/ve-dep-kieu-sa-cua-nu-dien-vien-vuong-tin-don-hen-ho-iker-casillas-ar706129.html</t>
+          <t>https://vtc.vn/12-tac-hai-cua-do-an-nhanh-voi-suc-khoe-ar687529.html</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>CAIiEN4tAKeMGgZOAFW93DpaKQkqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6ZDLBg</t>
+          <t>CAIiEF87UR0AZVMHmgXAPA5qVfwqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Mon, 10 Oct 2022 02:55:00 GMT</t>
+          <t>Wed, 13 Jul 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Vẻ đẹp kiêu sa của nữ diễn viên vướng tin đồn hẹn hò Iker Casillas  VTC News</t>
+          <t>12 tác hại của đồ ăn nhanh với sức khỏe  VTC News</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2565,32 +2565,32 @@
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr">
         <is>
-          <t>HLV Pipob: 'Thái Lan có vấn đề trong đào tạo trẻ' - VnExpress</t>
+          <t>Sức khỏe bé gái 18 tháng tuổi nghi bị bạo hành tại Hà Nội giờ thế nào? - VTC News</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hlv-pipob-thai-lan-dang-co-van-de-trong-dao-tao-tre-4521112.html</t>
+          <t>https://vtc.vn/suc-khoe-be-gai-18-thang-tuoi-nghi-bi-bao-hanh-tai-ha-noi-gio-the-nao-ar691366.html</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>CAIiEAguG2GPc0HLO-zoLOn7HvkqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiELkICQcna1NuQ5uI-2UhAygqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Sun, 09 Oct 2022 15:21:00 GMT</t>
+          <t>Mon, 01 Aug 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>HLV Pipob: 'Thái Lan có vấn đề trong đào tạo trẻ'  VnExpress</t>
+          <t>Sức khỏe bé gái 18 tháng tuổi nghi bị bạo hành tại Hà Nội giờ thế nào?  VTC News</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2601,27 +2601,27 @@
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Thị trường bất động sản 'đói' vốn: HoREA đề xuất nới room tín dụng thêm 1 - 2% - VTC News</t>
+          <t>12 vấn đề sức khỏe cần lưu ý ở những người ngoài 50 tuổi - VTC News</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>https://vtc.vn/thi-truong-bat-dong-san-doi-von-horea-de-xuat-no-i-room-ti-n-du-ng-them-1-2-ar706208.html</t>
+          <t>https://vtc.vn/12-van-de-suc-khoe-can-luu-y-o-nhung-nguoi-ngoai-50-tuoi-ar705984.html</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>CAIiEKikt_WPZYRbgnsl-I-nxV4qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww75DLBg</t>
+          <t>CAIiEFLxYyQoy3Zxq4KZEVCQzmMqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Sun, 09 Oct 2022 17:48:45 GMT</t>
+          <t>Sun, 09 Oct 2022 03:01:59 GMT</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Thị trường bất động sản 'đói' vốn: HoREA đề xuất nới room tín dụng thêm 1 - 2%  VTC News</t>
+          <t>12 vấn đề sức khỏe cần lưu ý ở những người ngoài 50 tuổi  VTC News</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -2637,32 +2637,32 @@
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Phóng viên CNN bị điều tra khi đưa tin vụ thảm sát ở Thái Lan - VnExpress</t>
+          <t>Sức khoẻ bé gái 3 tuổi ở Hà Nội bị đinh ghim vào đầu hiện thế nào? - VTC News</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/phong-vien-cnn-bi-dieu-tra-vi-dua-tin-vu-tham-sat-o-thai-lan-4521065.html</t>
+          <t>https://vtc.vn/suc-khoe-be-gai-3-tuoi-o-ha-noi-bi-dinh-ghim-vao-dau-hien-the-nao-ar661238.html</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>CAIiEPfp7COXF4-zgwisyzhKNgoqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEHUo1qSJZz_K_O2SxkPPeH8qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Sun, 09 Oct 2022 10:43:11 GMT</t>
+          <t>Mon, 14 Feb 2022 08:00:00 GMT</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Phóng viên CNN bị điều tra khi đưa tin vụ thảm sát ở Thái Lan  VnExpress</t>
+          <t>Sức khoẻ bé gái 3 tuổi ở Hà Nội bị đinh ghim vào đầu hiện thế nào?  VTC News</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2673,32 +2673,32 @@
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11thực phẩm phòng cảm cúm khi giao mùa - VnExpress</t>
+          <t>Dova Group hướng tới những sản phẩm chăm sóc sức khỏe phụ nữ - VTC News</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/11thuc-pham-phong-cam-cum-khi-giao-mua-4521015.html</t>
+          <t>https://vtc.vn/dova-group-huong-toi-nhung-san-pham-cham-soc-suc-khoe-phu-nu-ar696052.html</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>CAIiECcMX_Tv2UGnosvT35bpP78qMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwvs3WBg</t>
+          <t>CAIiEPhbmseZveA23kqpm_epVHYqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Sun, 09 Oct 2022 06:11:26 GMT</t>
+          <t>Mon, 22 Aug 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>11thực phẩm phòng cảm cúm khi giao mùa  VnExpress</t>
+          <t>Dova Group hướng tới những sản phẩm chăm sóc sức khỏe phụ nữ  VTC News</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2709,32 +2709,32 @@
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Ôtô bị lũ cuốn trôi 10 km - VnExpress</t>
+          <t>Bài tập chống đẩy tiết lộ nhiều bí mật sức khỏe nam giới, kể cả dự báo bệnh tim - VTC News</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/oto-bi-lu-cuon-troi-10-km-4520885.html</t>
+          <t>https://vtc.vn/bai-tap-chong-day-tiet-lo-nhieu-bi-mat-suc-khoe-nam-gioi-ke-ca-du-bao-benh-tim-ar684923.html</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>CAIiEELJThlpqyaeadXPiaa-7LMqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEG74hv9vCs2IgVmtHunbeUgqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Sat, 08 Oct 2022 14:10:00 GMT</t>
+          <t>Thu, 30 Jun 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Ôtô bị lũ cuốn trôi 10 km  VnExpress</t>
+          <t>Bài tập chống đẩy tiết lộ nhiều bí mật sức khỏe nam giới, kể cả dự báo bệnh tim  VTC News</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2745,32 +2745,32 @@
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Học lịch sử qua tour tham quan di sản - VnExpress</t>
+          <t>Ông Biden cập nhật tình hình sức khỏe sau khi mắc COVID-19 - VTC News</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hoc-lich-su-qua-tour-tham-quan-di-san-4520614.html</t>
+          <t>https://vtc.vn/ong-biden-cap-nhat-tinh-hinh-suc-khoe-sau-khi-mac-covid-19-ar689481.html</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>CAIiEMs1oztPiB7u_604-TraJZkqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEDWbf3DXc8hbI0aX8puw8_MqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Sat, 08 Oct 2022 02:27:00 GMT</t>
+          <t>Fri, 22 Jul 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Học lịch sử qua tour tham quan di sản  VnExpress</t>
+          <t>Ông Biden cập nhật tình hình sức khỏe sau khi mắc COVID-19  VTC News</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2781,32 +2781,32 @@
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Người đàn ông được cứu sống sau khi uống hơn 100 viên thuốc - VnExpress</t>
+          <t>5 dấu hiệu trên mặt cảnh báo sức khỏe lá lách, dạ dày đang xấu đi từng ngày - VTC News</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nguoi-dan-ong-duoc-cuu-song-sau-khi-uong-hon-100-vien-thuoc-4520244.html</t>
+          <t>https://vtc.vn/5-dau-hieu-tren-mat-canh-bao-suc-khoe-la-lach-da-day-dang-xau-di-tung-ngay-ar678795.html</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>CBMiXmh0dHBzOi8vdm5leHByZXNzLm5ldC9uZ3VvaS1kYW4tb25nLWR1b2MtY3V1LXNvbmctc2F1LWtoaS11b25nLWhvbi0xMDAtdmllbi10aHVvYy00NTIwMjQ0Lmh0bWzSAQA</t>
+          <t>CAIiEICPJ4fEV_BOVW49sPcUgs0qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Fri, 07 Oct 2022 03:49:02 GMT</t>
+          <t>Wed, 01 Jun 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Người đàn ông được cứu sống sau khi uống hơn 100 viên thuốc  VnExpress</t>
+          <t>5 dấu hiệu trên mặt cảnh báo sức khỏe lá lách, dạ dày đang xấu đi từng ngày  VTC News</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2817,32 +2817,32 @@
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Quan chức Lầu Năm Góc dự đoán Nga thất bại lớn ở Kherson - VnExpress</t>
+          <t>Màu nước tiểu tiết lộ gì về sức khỏe? - VTC News</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/quan-chuc-lau-nam-goc-du-doan-nga-that-bai-lon-o-kherson-4519099.html</t>
+          <t>https://vtc.vn/mau-nuoc-tieu-tiet-lo-gi-ve-suc-khoe-ar683586.html</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>CAIiEF3FcMKLsMf86mQR1a6nCOQqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwuM3WBg</t>
+          <t>CAIiEDEhxIZH7IjYf9N-DetmcJwqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Tue, 04 Oct 2022 07:00:00 GMT</t>
+          <t>Wed, 22 Jun 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Quan chức Lầu Năm Góc dự đoán Nga thất bại lớn ở Kherson  VnExpress</t>
+          <t>Màu nước tiểu tiết lộ gì về sức khỏe?  VTC News</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2853,27 +2853,27 @@
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Bản hợp đồng giữa học sinh lớp 4 và bố gây sốt cộng đồng mạng - VTC News</t>
+          <t>Cách đi bộ tạo nên 'kỳ tích' sức khỏe và tuổi thọ: Sớm áp dụng sẽ rất khỏe mạnh - VTC News</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>https://vtc.vn/ban-hop-dong-giua-hoc-sinh-lop-4-va-bo-gay-sot-cong-dong-mang-ar705435.html</t>
+          <t>https://vtc.vn/cach-di-bo-tao-nen-ky-tich-suc-khoe-va-tuoi-tho-som-ap-dung-se-rat-khoe-manh-ar665834.html</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>CAIiED68bJVAZfZsmoF6P6aHVZUqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEKCDlgSfVx3PNWLuDzLjSusqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Thu, 06 Oct 2022 08:00:00 GMT</t>
+          <t>Mon, 14 Mar 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Bản hợp đồng giữa học sinh lớp 4 và bố gây sốt cộng đồng mạng  VTC News</t>
+          <t>Cách đi bộ tạo nên 'kỳ tích' sức khỏe và tuổi thọ: Sớm áp dụng sẽ rất khỏe mạnh  VTC News</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -2889,32 +2889,32 @@
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr">
         <is>
-          <t>'Blonde': Sự tuyệt vọng của Marilyn Monroe - VnExpress</t>
+          <t>Cách ăn uống quyết định sức khỏe và tuổi thọ: Vì sao nên áp dụng từ khi còn trẻ? - VTC News</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/giai-tri/phim/thu-vien-phim/blonde-495</t>
+          <t>https://vtc.vn/cach-an-uong-quyet-dinh-suc-khoe-va-tuoi-tho-vi-sao-nen-ap-dung-tu-khi-con-tre-ar666084.html</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>CAIiEEzArUYP2xKGrzrMuTy3eg4qMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEDUL4njJRY27eOXjkGdsE94qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Wed, 05 Oct 2022 12:00:00 GMT</t>
+          <t>Tue, 15 Mar 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>'Blonde': Sự tuyệt vọng của Marilyn Monroe  VnExpress</t>
+          <t>Cách ăn uống quyết định sức khỏe và tuổi thọ: Vì sao nên áp dụng từ khi còn trẻ?  VTC News</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2925,27 +2925,27 @@
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Sản phẩm Thải độc gan thế hệ mới đạt Huy chương vàng vì sức khỏe cộng đồng - VTC News</t>
+          <t>HLV Petrovic vắng mặt 2 tuần vì lý do sức khoẻ - VTC News</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>https://vtc.vn/san-pham-thai-doc-gan-the-he-moi-dat-huy-chuong-vang-vi-suc-khoe-cong-dong-ar705366.html</t>
+          <t>https://vtc.vn/hlv-petrovic-vang-mat-2-tuan-vi-ly-do-suc-khoe-ar697346.html</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>CAIiEM7H3DyDGLfdloPx-8lI9eAqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
+          <t>CAIiEHAJpa-q7D01ljpnhz8R4n8qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Thu, 06 Oct 2022 02:11:00 GMT</t>
+          <t>Sun, 28 Aug 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Sản phẩm Thải độc gan thế hệ mới đạt Huy chương vàng vì sức khỏe cộng đồng  VTC News</t>
+          <t>HLV Petrovic vắng mặt 2 tuần vì lý do sức khoẻ  VTC News</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -2961,32 +2961,32 @@
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Học sinh, sinh viên Quảng Ninh đội mưa chạy S-Race - VnExpress</t>
+          <t>Những sai lầm trong bữa ăn sáng không tốt cho sức khỏe - VTC News</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hoc-sinh-sinh-vien-quang-ninh-doi-mua-chay-s-race-4519413.html</t>
+          <t>https://vtc.vn/nhung-sai-lam-trong-bua-an-sang-khong-tot-cho-suc-khoe-ar662461.html</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>CBMiVGh0dHBzOi8vdm5leHByZXNzLm5ldC9ob2Mtc2luaC1zaW5oLXZpZW4tcXVhbmctbmluaC1kb2ktbXVhLWNoYXktcy1yYWNlLTQ1MTk0MTMuaHRtbNIBAA</t>
+          <t>CAIiEHmcyoaeAKCRL1Rbyd9aFXwqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Mon, 03 Oct 2022 07:00:00 GMT</t>
+          <t>Tue, 22 Feb 2022 08:00:00 GMT</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Học sinh, sinh viên Quảng Ninh đội mưa chạy S-Race  VnExpress</t>
+          <t>Những sai lầm trong bữa ăn sáng không tốt cho sức khỏe  VTC News</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -2997,32 +2997,32 @@
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr">
         <is>
-          <t>BIDV ưu đãi cho khách khu vực Tây Nguyên - VnExpress</t>
+          <t>Làm gì để hồi phục sức khỏe nhanh sau khi mắc COVID-19? - VTC News</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/bidv-uu-dai-cho-khach-khu-vuc-tay-nguyen-4518701.html</t>
+          <t>https://vtc.vn/lam-gi-de-hoi-phuc-suc-khoe-nhanh-sau-khi-mac-covid-19-ar666695.html</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>CAIiEKXTcve4ezbyCYJ9clWmmGEqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEDm_uDlQbXP7yjj3z8mW4ZAqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Mon, 03 Oct 2022 07:00:00 GMT</t>
+          <t>Fri, 18 Mar 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>BIDV ưu đãi cho khách khu vực Tây Nguyên  VnExpress</t>
+          <t>Làm gì để hồi phục sức khỏe nhanh sau khi mắc COVID-19?  VTC News</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3033,32 +3033,32 @@
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Những dấu hiệu cơ thể thiếu vitamin A - VnExpress</t>
+          <t>Bạn gái của Hoàng Đức diện bikini khoe dáng nóng bỏng ở bờ biển Phú Quốc - VTC News</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nhung-dau-hieu-co-the-thieu-vitamin-a-4518457.html</t>
+          <t>https://vtc.vn/ban-gai-cua-hoang-duc-dien-bikini-khoe-dang-nong-bong-o-bo-bien-phu-quoc-ar704193.html</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>CAIiEJgA3bW14saO48eKu8_rGd4qMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwvs3WBg</t>
+          <t>CBMiZWh0dHBzOi8vdnRjLnZuL2Jhbi1nYWktY3VhLWhvYW5nLWR1Yy1kaWVuLWJpa2luaS1raG9lLWRhbmctbm9uZy1ib25nLW8tYm8tYmllbi1waHUtcXVvYy1hcjcwNDE5My5odG1s0gFpaHR0cHM6Ly9hbXAudnRjLnZuL2Jhbi1nYWktY3VhLWhvYW5nLWR1Yy1kaWVuLWJpa2luaS1raG9lLWRhbmctbm9uZy1ib25nLW8tYm8tYmllbi1waHUtcXVvYy1hcjcwNDE5My5odG1s</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Mon, 03 Oct 2022 07:00:00 GMT</t>
+          <t>Fri, 30 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Những dấu hiệu cơ thể thiếu vitamin A  VnExpress</t>
+          <t>Bạn gái của Hoàng Đức diện bikini khoe dáng nóng bỏng ở bờ biển Phú Quốc  VTC News</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3069,32 +3069,32 @@
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Ôtô khách bị ném đá - VnExpress</t>
+          <t>Cộng đồng yêu xe hào hứng 'khoe' vé đại nhạc hội VinFast - VTC News</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/oto-khach-bi-nem-da-4517675.html</t>
+          <t>https://vtc.vn/cong-dong-yeu-xe-hao-hung-khoe-ve-dai-nhac-hoi-vinfast-ar705032.html</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>CAIiENm0pjAqAyLqgmVxKIsYZaUqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwt83WBg</t>
+          <t>CAIiEPLpuOLWZGPJsChj600OTC8qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7JDLBg</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Fri, 30 Sep 2022 07:00:00 GMT</t>
+          <t>Tue, 04 Oct 2022 07:50:00 GMT</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Ôtô khách bị ném đá  VnExpress</t>
+          <t>Cộng đồng yêu xe hào hứng 'khoe' vé đại nhạc hội VinFast  VTC News</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3105,32 +3105,32 @@
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Cô gái sống đơn giản, yêu ghét rõ ràng - VnExpress</t>
+          <t>6 vấn đề sức khỏe biểu hiện qua móng tay: Quan sát hàng ngày giúp phát hiện bệnh - VTC News</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/co-gai-song-don-gian-yeu-ghet-ro-rang-4517259.html</t>
+          <t>https://vtc.vn/6-van-de-suc-khoe-bieu-hien-qua-mong-tay-ar657915.html</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>CAIiEHBkMi2gU4e2oCceobBVaJoqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEEyGrfw6krjOkBg2ANitgp0qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Thu, 29 Sep 2022 07:00:00 GMT</t>
+          <t>Fri, 21 Jan 2022 08:00:00 GMT</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Cô gái sống đơn giản, yêu ghét rõ ràng  VnExpress</t>
+          <t>6 vấn đề sức khỏe biểu hiện qua móng tay: Quan sát hàng ngày giúp phát hiện bệnh  VTC News</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3141,32 +3141,32 @@
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Lý do ông Putin không phát lệnh tổng động viên - VnExpress</t>
+          <t>Tặng 100.000 thực phẩm bảo vệ sức khỏe Kiện Cốt Vương cho người bệnh xương khớp - VTC News</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ly-do-ong-putin-khong-phat-lenh-tong-dong-vien-4514097.html</t>
+          <t>https://vtc.vn/tang-100-000-thuc-pham-bao-ve-suc-khoe-kien-cot-vuong-cho-nguoi-benh-xuong-khop-ar686650.html</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>CAIiEPeD4tvUW9Fvm7EI0nnLliUqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwuM3WBg</t>
+          <t>CAIiEDAWSpuRc8KG099Pem0P9_oqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Thu, 22 Sep 2022 07:00:00 GMT</t>
+          <t>Fri, 08 Jul 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Lý do ông Putin không phát lệnh tổng động viên  VnExpress</t>
+          <t>Tặng 100.000 thực phẩm bảo vệ sức khỏe Kiện Cốt Vương cho người bệnh xương khớp  VTC News</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3177,32 +3177,32 @@
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Kết quả U20 Việt Nam vs U20 Indonesia: Việt Nam thua ngược 2-3 - VnExpress</t>
+          <t>Nga bác tin đồn về sức khỏe của Tổng thống Putin - VTC News</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/u20-viet-nam-vs-u20-indonesia-4512802-tong-thuat.html</t>
+          <t>https://vtc.vn/nga-bac-tin-don-ve-suc-khoe-cua-tong-thong-putin-ar689433.html</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>CAIiEPawM6nSHjQbrnfQD7Y5zcoqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwu83WBg</t>
+          <t>CAIiEA3rfAXBj5MzlhiA5FjYlyoqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwhJDLBg</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Sun, 18 Sep 2022 07:00:00 GMT</t>
+          <t>Thu, 21 Jul 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Kết quả U20 Việt Nam vs U20 Indonesia: Việt Nam thua ngược 2-3  VnExpress</t>
+          <t>Nga bác tin đồn về sức khỏe của Tổng thống Putin  VTC News</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3213,32 +3213,32 @@
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Hàng trăm người tham dự triển lãm cưới tại Furama Resort Đà Nẵng - VnExpress</t>
+          <t>4 người tử vong ở Công ty Miwon: Sức khoẻ của người sống sót chuyển biến xấu - VTC News</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hang-tram-nguoi-tham-du-trien-lam-cuoi-tai-furama-resort-da-nang-4522321.html</t>
+          <t>https://vtc.vn/4-nguoi-tu-vong-o-cong-ty-miwon-suc-khoe-cua-nguoi-song-sot-chuyen-bien-xau-ar689172.html</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>CAIiEAtT86_vNcf54Xqgfr8OMGMqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEOqAuuWaDDrOdeEFIH009KEqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww84TLBg</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Wed, 12 Oct 2022 00:00:00 GMT</t>
+          <t>Wed, 20 Jul 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Hàng trăm người tham dự triển lãm cưới tại Furama Resort Đà Nẵng  VnExpress</t>
+          <t>4 người tử vong ở Công ty Miwon: Sức khoẻ của người sống sót chuyển biến xấu  VTC News</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3249,32 +3249,32 @@
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Bộ Giáo dục mở hệ thống xác nhận nhập học từ hôm nay - VnExpress</t>
+          <t>Sức khỏe 34 du khách bị ngộ độc thực phẩm ở Đà Nẵng hiện ra sao? - VTC News</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/bo-giao-duc-mo-he-thong-xac-nhan-nhap-hoc-tu-hom-nay-4512695.html</t>
+          <t>https://vtc.vn/suc-khoe-34-du-khach-bi-ngo-doc-thuc-pham-o-da-nang-hien-ra-sao-ar691879.html</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>CAIiEO2n6RzNOAV5xBsz_uNOBGAqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwvc3WBg</t>
+          <t>CAIiENsTu21s6eCX0kVykpawj2QqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Sun, 18 Sep 2022 07:00:00 GMT</t>
+          <t>Wed, 03 Aug 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Bộ Giáo dục mở hệ thống xác nhận nhập học từ hôm nay  VnExpress</t>
+          <t>Sức khỏe 34 du khách bị ngộ độc thực phẩm ở Đà Nẵng hiện ra sao?  VTC News</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3285,32 +3285,32 @@
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Điểm tin 29/9: Nữ MC khoá Facebook sau phát ngôn 'đón bão ra hồn bão' - Ngôi Sao</t>
+          <t>Người trẻ mờ mắt, suy thận vì căn bệnh âm thầm tàn phá sức khoẻ - VTC News</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>https://ngoisao.vnexpress.net/video/diem-tin-29-9-nu-mc-khoa-facebook-sau-phat-ngon-don-bao-ra-hon-bao-4517000.html</t>
+          <t>https://vtc.vn/nguoi-tre-mo-mat-suy-than-vi-can-benh-am-tham-tan-pha-suc-khoe-ar694428.html</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>CAIiEGC0uE0VbH71_ZbbqFgC6AIqMwgEKioIACIQyq3Fh2mV-aXM5A3HYfBoBioUCAoiEMqtxYdplfmlzOQNx2HwaAYwsKvYBg</t>
+          <t>CAIiEO_2B533HDMs-Cj0KSl3fMsqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Thu, 29 Sep 2022 07:00:00 GMT</t>
+          <t>Mon, 15 Aug 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Điểm tin 29/9: Nữ MC khoá Facebook sau phát ngôn 'đón bão ra hồn bão'  Ngôi Sao</t>
+          <t>Người trẻ mờ mắt, suy thận vì căn bệnh âm thầm tàn phá sức khoẻ  VTC News</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Ngôi Sao</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3321,32 +3321,32 @@
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Nghị sĩ mang ngựa vào tòa quốc hội - VnExpress</t>
+          <t>Công dụng bất ngờ của Platin với sức khỏe - VTC News</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nghi-si-mang-ngua-vao-toa-quoc-hoi-4517012.html</t>
+          <t>https://vtc.vn/cong-dung-bat-ngo-cua-platin-voi-suc-khoe-ar672836.html</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>CAIiEKEZ3hA9oQDDy5oXalL5QVIqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwuM3WBg</t>
+          <t>CAIiEN0Dca6xEZIlRRf8QO1T3h0qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Thu, 29 Sep 2022 07:00:00 GMT</t>
+          <t>Fri, 22 Apr 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Nghị sĩ mang ngựa vào tòa quốc hội  VnExpress</t>
+          <t>Công dụng bất ngờ của Platin với sức khỏe  VTC News</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3357,32 +3357,32 @@
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Điểm chuẩn Học viện Tài chính (AOF) 2022 - VnExpress</t>
+          <t>Á hậu Kim Duyên: 'Sức khỏe tinh thần của tôi đang hoàn toàn không tốt' - VTC News</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/diem-chuan-hoc-vien-tai-chinh-giam-4511613.html</t>
+          <t>https://vtc.vn/a-hau-kim-duyen-suc-khoe-tinh-than-cua-toi-dang-hoan-toan-khong-tot-ar692409.html</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>CAIiEFKy7KS3gUXwXJXW1gHryTUqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwvc3WBg</t>
+          <t>CAIiEI14I30_ofJsQ_VEmEYtla8qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Fri, 16 Sep 2022 07:00:00 GMT</t>
+          <t>Fri, 05 Aug 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Điểm chuẩn Học viện Tài chính (AOF) 2022  VnExpress</t>
+          <t>Á hậu Kim Duyên: 'Sức khỏe tinh thần của tôi đang hoàn toàn không tốt'  VTC News</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3393,27 +3393,27 @@
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Lịch thi đấu của tuyển Việt Nam tại giải giao hữu quốc tế 2022 - VTC News</t>
+          <t>Chuyển giao đạm thủy phân Liver Hi - bước tiến vì sức khỏe cộng đồng - VTC News</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>https://vtc.vn/lich-thi-dau-cua-tuyen-viet-nam-tai-giai-giao-huu-quoc-te-2022-ar701809.html</t>
+          <t>https://vtc.vn/chuyen-giao-dam-thuy-phan-liver-hi-buoc-tien-vi-suc-khoe-cong-dong-ar680394.html</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>CAIiEJHF5Ey2Ozex7M2pun8c_AgqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6ZDLBg</t>
+          <t>CAIiEG9gZgJqr38V5yHaNl9Qt1wqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Mon, 19 Sep 2022 07:00:00 GMT</t>
+          <t>Fri, 03 Jun 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Lịch thi đấu của tuyển Việt Nam tại giải giao hữu quốc tế 2022  VTC News</t>
+          <t>Chuyển giao đạm thủy phân Liver Hi - bước tiến vì sức khỏe cộng đồng  VTC News</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -3429,32 +3429,32 @@
       <c r="B84" t="inlineStr"/>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Nghe podcasts | Điểm tin 21h: 5 sân bay dừng khai thác do bão; USD ngân hàng lên sát 23.900 đồng - VnExpress</t>
+          <t>Phòng khám đa khoa Hữu Nghị tại Đà Nẵng - nơi gửi gắm sức khỏe của mọi người - VTC News</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/diem-tin-21h-5-san-bay-dung-khai-thac-do-bao-usd-ngan-hang-len-sat-23-900-dong-4515619.html</t>
+          <t>https://vtc.vn/phong-kham-da-khoa-huu-nghi-tai-da-nang-noi-gui-gam-suc-khoe-cua-moi-nguoi-ar688925.html</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>CBMicWh0dHBzOi8vdm5leHByZXNzLm5ldC9kaWVtLXRpbi0yMWgtNS1zYW4tYmF5LWR1bmcta2hhaS10aGFjLWRvLWJhby11c2Qtbmdhbi1oYW5nLWxlbi1zYXQtMjMtOTAwLWRvbmctNDUxNTYxOS5odG1s0gEA</t>
+          <t>CAIiEAe7AJZzoGx9sy779Ww5kysqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Mon, 26 Sep 2022 07:00:00 GMT</t>
+          <t>Tue, 19 Jul 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Nghe podcasts | Điểm tin 21h: 5 sân bay dừng khai thác do bão; USD ngân hàng lên sát 23.900 đồng  VnExpress</t>
+          <t>Phòng khám đa khoa Hữu Nghị tại Đà Nẵng - nơi gửi gắm sức khỏe của mọi người  VTC News</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3465,32 +3465,32 @@
       <c r="B85" t="inlineStr"/>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Hàng nghìn khán giả nghe Tuấn Hưng hát từ ban công - VnExpress</t>
+          <t>Đàm Vĩnh Hưng khoe nhận được quà sinh nhật đặc biệt từ fan hâm mộ - VTC News</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hang-nghin-khan-gia-nghe-tuan-hung-hat-tu-ban-cong-4515480.html</t>
+          <t>https://vtc.vn/dam-vinh-hung-khoe-nhan-duoc-qua-sinh-nhat-dac-biet-tu-fan-ham-mo-ar703484.html</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>CAIiEEohB5VhzqkR-YxCaaDEvSUqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwus3WBg</t>
+          <t>CBMiXmh0dHBzOi8vdnRjLnZuL2RhbS12aW5oLWh1bmcta2hvZS1uaGFuLWR1b2MtcXVhLXNpbmgtbmhhdC1kYWMtYmlldC10dS1mYW4taGFtLW1vLWFyNzAzNDg0Lmh0bWzSAWJodHRwczovL2FtcC52dGMudm4vZGFtLXZpbmgtaHVuZy1raG9lLW5oYW4tZHVvYy1xdWEtc2luaC1uaGF0LWRhYy1iaWV0LXR1LWZhbi1oYW0tbW8tYXI3MDM0ODQuaHRtbA</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Sun, 25 Sep 2022 07:00:00 GMT</t>
+          <t>Tue, 27 Sep 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Hàng nghìn khán giả nghe Tuấn Hưng hát từ ban công  VnExpress</t>
+          <t>Đàm Vĩnh Hưng khoe nhận được quà sinh nhật đặc biệt từ fan hâm mộ  VTC News</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3501,32 +3501,32 @@
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Những bước Anh chuẩn bị cho triều đại Vua Charles III - VnExpress</t>
+          <t>Cảnh báo quảng cáo sản phẩm bảo vệ sức khỏe Lumedi-V,Lumedi–V KISD trên facebook - VTC News</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nhung-buoc-anh-chuan-bi-cho-trieu-dai-vua-charles-iii-4512933.html</t>
+          <t>https://vtc.vn/canh-bao-quang-cao-san-pham-bao-ve-suc-khoe-lumedi-v-lumedi-v-kisd-tren-facebook-ar676013.html</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>CAIiEHACSFUTmPnQkP2xMxr9nQYqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw1KzYBg</t>
+          <t>CAIiEO-084R-NXrHnc4S9VYp8KkqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Tue, 20 Sep 2022 07:00:00 GMT</t>
+          <t>Wed, 11 May 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Những bước Anh chuẩn bị cho triều đại Vua Charles III  VnExpress</t>
+          <t>Cảnh báo quảng cáo sản phẩm bảo vệ sức khỏe Lumedi-V,Lumedi–V KISD trên facebook  VTC News</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3537,32 +3537,32 @@
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Apple xác nhận lỗi lạ trên bộ đôi iPhone 14 Pro - VnExpress</t>
+          <t>Giấy bạc bọc thực phẩm có gây hại sức khỏe? - VTC News</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/apple-xac-nhan-loi-la-tren-bo-doi-iphone-14-pro-4513423.html</t>
+          <t>https://vtc.vn/giay-bac-boc-thuc-pham-co-gay-hai-suc-khoe-ar673558.html</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>CAIiEM96zNy6E9JNfXvlhL3deb0qMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwws3WBg</t>
+          <t>CAIiEMWaZnBZ-D1WC-BmCsXrJdUqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Tue, 20 Sep 2022 07:00:00 GMT</t>
+          <t>Wed, 27 Apr 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Apple xác nhận lỗi lạ trên bộ đôi iPhone 14 Pro  VnExpress</t>
+          <t>Giấy bạc bọc thực phẩm có gây hại sức khỏe?  VTC News</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3573,27 +3573,27 @@
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr">
         <is>
-          <t>6 ca tử vong do virus Adeno, Bộ Y tế yêu cầu không để bùng dịch - VTC News</t>
+          <t>Sức khỏe 4 người được cứu trong vụ 15 ngư dân mất tích trên biển hiện rất yếu - VTC News</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>https://vtc.vn/6-ca-tu-vong-do-virus-adeno-bo-y-te-yeu-cau-khong-de-bung-dich-ar702251.html</t>
+          <t>https://vtc.vn/15-ngu-dan-mat-tich-tren-bien-suc-khoe-4-nguoi-duoc-cuu-dang-rat-yeu-ar689062.html</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>CAIiEJl3txcZAri4GD2pOxpUp7YqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEAPPrec3kuR30q-xuSZCHb4qMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww84TLBg</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Wed, 21 Sep 2022 07:00:00 GMT</t>
+          <t>Wed, 20 Jul 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>6 ca tử vong do virus Adeno, Bộ Y tế yêu cầu không để bùng dịch  VTC News</t>
+          <t>Sức khỏe 4 người được cứu trong vụ 15 ngư dân mất tích trên biển hiện rất yếu  VTC News</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -3609,32 +3609,32 @@
       <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Hứng bóng, nuôi thú ảo với Dynamic Island - VnExpress</t>
+          <t>Giám đốc BV Lê Văn Thịnh: ‘Mong có thêm nhiều sức khỏe để chăm sóc người dân’ - VTC News</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hung-bong-nuoi-thu-ao-voi-dynamic-island-4512895.html</t>
+          <t>https://vtc.vn/giam-doc-bv-le-van-thinh-mong-co-them-nhieu-suc-khoe-de-cham-soc-nguoi-dan-ar663418.html</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>CAIiELnSg2wnQHlQugsWQJFOFYEqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwws3WBg</t>
+          <t>CAIiENj0mfkqGrpEvS7EqpWXZQwqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Mon, 19 Sep 2022 07:00:00 GMT</t>
+          <t>Sun, 27 Feb 2022 08:00:00 GMT</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Hứng bóng, nuôi thú ảo với Dynamic Island  VnExpress</t>
+          <t>Giám đốc BV Lê Văn Thịnh: ‘Mong có thêm nhiều sức khỏe để chăm sóc người dân’  VTC News</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3645,32 +3645,32 @@
       <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Ảnh sao 21/9: Phương Oanh và shark Bình tình tứ ở sự kiện - Ngôi Sao</t>
+          <t>Sức khỏe tụt dốc, NS Hoài Linh từng trải qua những căn bệnh nghiêm trọng nào? - VTC News</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>https://ngoisao.vnexpress.net/anh-sao-21-9-phuong-oanh-va-shark-binh-tinh-tu-o-su-kien-4513786.html</t>
+          <t>https://vtc.vn/suc-khoe-tut-doc-ns-hoai-linh-tung-trai-qua-nhung-can-benh-nghiem-trong-nao-ar656286.html</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>CAIiEGkbjRlj9LYZVXbcBi5mV1gqMwgEKioIACIQyq3Fh2mV-aXM5A3HYfBoBioUCAoiEMqtxYdplfmlzOQNx2HwaAYw_d3MBw</t>
+          <t>CBMiaGh0dHBzOi8vdnRjLnZuL3N1Yy1raG9lLXR1dC1kb2MtbnMtaG9haS1saW5oLXR1bmctdHJhaS1xdWEtbmh1bmctY2FuLWJlbmgtbmdoaWVtLXRyb25nLW5hby1hcjY1NjI4Ni5odG1s0gFsaHR0cHM6Ly9hbXAudnRjLnZuL3N1Yy1raG9lLXR1dC1kb2MtbnMtaG9haS1saW5oLXR1bmctdHJhaS1xdWEtbmh1bmctY2FuLWJlbmgtbmdoaWVtLXRyb25nLW5hby1hcjY1NjI4Ni5odG1s</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Wed, 21 Sep 2022 07:00:00 GMT</t>
+          <t>Sun, 09 Jan 2022 08:00:00 GMT</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Ảnh sao 21/9: Phương Oanh và shark Bình tình tứ ở sự kiện  Ngôi Sao</t>
+          <t>Sức khỏe tụt dốc, NS Hoài Linh từng trải qua những căn bệnh nghiêm trọng nào?  VTC News</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Ngôi Sao</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3681,32 +3681,32 @@
       <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Anh trai đăng 30 video cáo buộc Pogba - VnExpress</t>
+          <t>Không chỉ là gia vị, hành lá còn có tác dụng 'vàng' với sức khỏe bạn nên biết - VTC News</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/anh-trai-dang-30-video-cao-buoc-pogba-4515279.html</t>
+          <t>https://vtc.vn/khong-chi-la-gia-vi-hanh-la-con-co-tac-dung-vang-voi-suc-khoe-ban-nen-biet-ar683069.html</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>CAIiEHPjnYeiK0lhNATHGM4rPUwqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw0I3LBg</t>
+          <t>CAIiEFlGhjQkt06ys7j98vZcz3AqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Sat, 24 Sep 2022 07:00:00 GMT</t>
+          <t>Sun, 19 Jun 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Anh trai đăng 30 video cáo buộc Pogba  VnExpress</t>
+          <t>Không chỉ là gia vị, hành lá còn có tác dụng 'vàng' với sức khỏe bạn nên biết  VTC News</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3717,32 +3717,32 @@
       <c r="B92" t="inlineStr"/>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Cuộc sống trong hẻm phố Tây Sài Gòn - VnExpress</t>
+          <t>Chuyên gia khuyến cáo 3 sai lầm khi giảm cân: Vừa thất bại, vừa gây hại sức khỏe - VTC News</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/cuoc-song-trong-hem-pho-tay-sai-gon-4514371.html</t>
+          <t>https://vtc.vn/chuyen-gia-khuyen-cao-3-sai-lam-khi-giam-can-vua-that-bai-vua-gay-hai-suc-khoe-ar679871.html</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>CAIiEKRTqzBuxjqQh9wKqpP-AQAqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw1KzYBg</t>
+          <t>CAIiELzMN8KO3xv3HJrs6uXIVoQqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Sat, 24 Sep 2022 07:00:00 GMT</t>
+          <t>Fri, 03 Jun 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Cuộc sống trong hẻm phố Tây Sài Gòn  VnExpress</t>
+          <t>Chuyên gia khuyến cáo 3 sai lầm khi giảm cân: Vừa thất bại, vừa gây hại sức khỏe  VTC News</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3753,27 +3753,27 @@
       <c r="B93" t="inlineStr"/>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Phát hiện quả bom nặng gần 600kg khi xây cầu - VTC News</t>
+          <t>Á hậu Bảo Ngọc nổi bật trong phần thi bikini tại Hoa hậu Liên lục địa 2022 - VTC News</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>https://vtc.vn/phat-hien-qua-bom-nang-gan-600kg-khi-xay-cau-ar702728.html</t>
+          <t>https://vtc.vn/a-hau-bao-ngoc-noi-bat-trong-phan-thi-bikini-tai-hoa-hau-lien-luc-dia-2022-ar706653.html</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>CAIiEG_EvT3aXVya-w0sjkt3cSIqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww84TLBg</t>
+          <t>CAIiEG7OL_Xb0pHk07nDUscRjWQqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwh5DLBg</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Fri, 23 Sep 2022 07:00:00 GMT</t>
+          <t>Wed, 12 Oct 2022 02:46:00 GMT</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Phát hiện quả bom nặng gần 600kg khi xây cầu  VTC News</t>
+          <t>Á hậu Bảo Ngọc nổi bật trong phần thi bikini tại Hoa hậu Liên lục địa 2022  VTC News</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -3789,27 +3789,27 @@
       <c r="B94" t="inlineStr"/>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Tạm đình chỉ nữ giáo viên lấy gai bưởi châm vào tay trẻ mầm non - VTC News</t>
+          <t>7 thói quen giúp thận luôn khỏe mạnh - VTC News</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>https://vtc.vn/tam-dinh-chi-nu-giao-vien-lay-gai-buoi-cham-vao-tay-tre-mam-non-ar702358.html</t>
+          <t>https://vtc.vn/7-thoi-quen-giup-than-luon-khoe-manh-ar665355.html</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>CAIiEL0_28pdgPsOU4Id6qz5HZEqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
+          <t>CAIiEFUrrxCgJE0BXauP6PmjEmMqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Thu, 22 Sep 2022 07:00:00 GMT</t>
+          <t>Fri, 11 Mar 2022 08:00:00 GMT</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Tạm đình chỉ nữ giáo viên lấy gai bưởi châm vào tay trẻ mầm non  VTC News</t>
+          <t>7 thói quen giúp thận luôn khỏe mạnh  VTC News</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -3825,32 +3825,32 @@
       <c r="B95" t="inlineStr"/>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Triệu chứng nhiễm Adenovirus khác Covid, cảm thế nào - VnExpress</t>
+          <t>NovaWorld Phan Thiet: Mảnh ghép hoàn hảo cho du lịch chăm sóc sức khỏe Việt Nam - VTC News</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/trieu-chung-nhiem-adenovirus-khac-covid-cam-the-nao-4514773.html</t>
+          <t>https://vtc.vn/novaworld-phan-thiet-manh-ghep-hoan-hao-cho-du-lich-cham-soc-suc-khoe-viet-nam-ar665173.html</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>CAIiEHly4DkyIdIuU8rS-zsyU_EqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw1KzYBg</t>
+          <t>CBMia2h0dHBzOi8vdnRjLnZuL25vdmF3b3JsZC1waGFuLXRoaWV0LW1hbmgtZ2hlcC1ob2FuLWhhby1jaG8tZHUtbGljaC1jaGFtLXNvYy1zdWMta2hvZS12aWV0LW5hbS1hcjY2NTE3My5odG1s0gFvaHR0cHM6Ly9hbXAudnRjLnZuL25vdmF3b3JsZC1waGFuLXRoaWV0LW1hbmgtZ2hlcC1ob2FuLWhhby1jaG8tZHUtbGljaC1jaGFtLXNvYy1zdWMta2hvZS12aWV0LW5hbS1hcjY2NTE3My5odG1s</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Fri, 23 Sep 2022 07:00:00 GMT</t>
+          <t>Thu, 10 Mar 2022 08:00:00 GMT</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Triệu chứng nhiễm Adenovirus khác Covid, cảm thế nào  VnExpress</t>
+          <t>NovaWorld Phan Thiet: Mảnh ghép hoàn hảo cho du lịch chăm sóc sức khỏe Việt Nam  VTC News</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3861,32 +3861,32 @@
       <c r="B96" t="inlineStr"/>
       <c r="C96" t="inlineStr">
         <is>
-          <t>'Avatar' tập một được dự đoán thành phim đầu tiên cán mốc 3 tỷ USD - Ngôi Sao</t>
+          <t>Ăn táo thời điểm nào trong ngày là có lợi cho sức khoẻ nhất? - VTC News</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>https://ngoisao.vnexpress.net/avatar-tap-mot-duoc-du-doan-thanh-phim-dau-tien-can-moc-3-ty-usd-4514533.html</t>
+          <t>https://vtc.vn/an-tao-thoi-diem-nao-trong-ngay-la-co-loi-cho-suc-khoe-nhat-ar675751.html</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>CAIiEIKL6PTo1jlCL3D184oCrmwqMwgEKioIACIQyq3Fh2mV-aXM5A3HYfBoBioUCAoiEMqtxYdplfmlzOQNx2HwaAYwsKvYBg</t>
+          <t>CAIiEB6zfO2LHGNaMgCwjFXcZhAqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Thu, 22 Sep 2022 07:00:00 GMT</t>
+          <t>Tue, 10 May 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>'Avatar' tập một được dự đoán thành phim đầu tiên cán mốc 3 tỷ USD  Ngôi Sao</t>
+          <t>Ăn táo thời điểm nào trong ngày là có lợi cho sức khoẻ nhất?  VTC News</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Ngôi Sao</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3897,32 +3897,32 @@
       <c r="B97" t="inlineStr"/>
       <c r="C97" t="inlineStr">
         <is>
-          <t>'Big Mouth': Hành trình tìm công lý - VnExpress</t>
+          <t>Con gửi thư chúc sức khỏe kèm bức vẽ lạ, mẹ hốt hoảng ‘con không cần mẹ nữa sao’ - VTC News</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/giai-tri/phim/thu-vien-phim/big-mouth-489</t>
+          <t>https://vtc.vn/con-gui-thu-chuc-suc-khoe-kem-buc-ve-la-me-hot-hoang-con-khong-can-me-nua-sao-ar670975.html</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>CAIiEOENUPMoHqImklZM02bFlkAqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwus3WBg</t>
+          <t>CAIiEPxgOSaMGzgwYkLE9tXaeRIqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Thu, 22 Sep 2022 07:00:00 GMT</t>
+          <t>Tue, 12 Apr 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>'Big Mouth': Hành trình tìm công lý  VnExpress</t>
+          <t>Con gửi thư chúc sức khỏe kèm bức vẽ lạ, mẹ hốt hoảng ‘con không cần mẹ nữa sao’  VTC News</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3933,32 +3933,32 @@
       <c r="B98" t="inlineStr"/>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Lý do giá dầu lần đầu vượt xăng - VnExpress</t>
+          <t>Dự kiến ngưỡng xét tuyển đầu vào ngành sức khỏe, giáo viên năm 2022 - VTC News</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/vi-sao-gia-dau-cao-hon-xang-4507737.html</t>
+          <t>https://vtc.vn/du-kien-nguong-xet-tuyen-dau-vao-nganh-suc-khoe-giao-vien-nam-2022-ar671942.html</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>CAIiEE3uxvRMM4aFb9wxtGAIZTkqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgw1KzYBg</t>
+          <t>CAIiEKd9l2RGOc0uysav4QE1jhQqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww8oTLBg</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Tue, 06 Sep 2022 07:00:00 GMT</t>
+          <t>Mon, 18 Apr 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Lý do giá dầu lần đầu vượt xăng  VnExpress</t>
+          <t>Dự kiến ngưỡng xét tuyển đầu vào ngành sức khỏe, giáo viên năm 2022  VTC News</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -3969,27 +3969,27 @@
       <c r="B99" t="inlineStr"/>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Vietlott Power 6/55 22/9 - Trực tiếp kết quả xổ số Vietlott 22/9/2022 - VTC News</t>
+          <t>7 lợi ích tuyệt vời của magie với sức khỏe có thể bạn chưa biết - VTC News</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>https://vtc.vn/vietlott-power-6-55-22-9-truc-tiep-ket-qua-xo-so-vietlott-22-9-2022-ar702245.html</t>
+          <t>https://vtc.vn/7-loi-ich-tuyet-voi-cua-magie-voi-suc-khoe-co-the-ban-chua-biet-ar651550.html</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>CAIiEEDNKRcGzsfbkSeXo9dNQhIqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7wwkr_sBw</t>
+          <t>CAIiEOTpY_I6Zl2pLgWMRBqeaHcqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww6pDLBg</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Wed, 21 Sep 2022 07:00:00 GMT</t>
+          <t>Mon, 13 Dec 2021 08:00:00 GMT</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Vietlott Power 6/55 22/9 - Trực tiếp kết quả xổ số Vietlott 22/9/2022  VTC News</t>
+          <t>7 lợi ích tuyệt vời của magie với sức khỏe có thể bạn chưa biết  VTC News</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -4005,32 +4005,32 @@
       <c r="B100" t="inlineStr"/>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Ahn Jae Hyun ăn bánh căn vỉa hè ở Sài Gòn - Ngôi Sao</t>
+          <t>Nha khoa Quốc tế DAISY tổ chức Ngày hội sức khỏe răng miệng - VTC News</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>https://ngoisao.vnexpress.net/ahn-jae-hyun-an-banh-can-via-he-o-sai-gon-4514216.html</t>
+          <t>https://vtc.vn/nha-khoa-quoc-te-daisy-to-chuc-ngay-hoi-suc-khoe-rang-mieng-ar667961.html</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>CAIiEAhqU7GNbeoH5ehNXL4_cbIqMwgEKioIACIQyq3Fh2mV-aXM5A3HYfBoBioUCAoiEMqtxYdplfmlzOQNx2HwaAYwr6vYBg</t>
+          <t>CAIiEFqY9cj96CZxQ6uIxQUdycEqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww7pDLBg</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Thu, 22 Sep 2022 07:00:00 GMT</t>
+          <t>Fri, 25 Mar 2022 07:00:00 GMT</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Ahn Jae Hyun ăn bánh căn vỉa hè ở Sài Gòn  Ngôi Sao</t>
+          <t>Nha khoa Quốc tế DAISY tổ chức Ngày hội sức khỏe răng miệng  VTC News</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>Ngôi Sao</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>
@@ -4041,32 +4041,32 @@
       <c r="B101" t="inlineStr"/>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Hơn 2,5 triệu người Việt không biết mình bệnh tiểu đường - VnExpress</t>
+          <t>Ông nội thông tin về sức khỏe bé gái 3 tuổi bị găm đinh vào đầu - VTC News</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hon-2-5-trieu-nguoi-viet-khong-biet-minh-benh-tieu-duong-4514043.html</t>
+          <t>https://vtc.vn/ong-noi-thong-tin-ve-suc-khoe-be-gai-3-tuoi-bi-gam-dinh-vao-dau-ar658869.html</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>CAIiEPrVguACKjpFMkD2F-q3xnAqMwgEKioIACIQAMXzVBQHxZVyYLLE6HuReCoUCAoiEADF81QUB8WVcmCyxOh7kXgwvs3WBg</t>
+          <t>CAIiEDxP3_AY8f6BEJdpWPf_xcYqMwgEKioIACIQSeNkRqBVIknN-UrQuAOrvCoUCAoiEEnjZEagVSJJzflK0LgDq7ww84TLBg</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Wed, 21 Sep 2022 07:00:00 GMT</t>
+          <t>Wed, 26 Jan 2022 08:00:00 GMT</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Hơn 2,5 triệu người Việt không biết mình bệnh tiểu đường  VnExpress</t>
+          <t>Ông nội thông tin về sức khỏe bé gái 3 tuổi bị găm đinh vào đầu  VTC News</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>VnExpress</t>
+          <t>VTC News</t>
         </is>
       </c>
     </row>

</xml_diff>